<commit_message>
Activity state and ejection from memory
</commit_message>
<xml_diff>
--- a/doc/android.xlsx
+++ b/doc/android.xlsx
@@ -3,28 +3,29 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11014"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F6C482-75C6-404C-AD5B-F4B2EF443B71}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9906F8-A00B-584A-B469-F1A6AD0199F9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Activity_Lifecycle" sheetId="15" r:id="rId1"/>
-    <sheet name="ContentProvider" sheetId="4" r:id="rId2"/>
-    <sheet name="Android高级应用开发-深入篇" sheetId="5" r:id="rId3"/>
-    <sheet name="反编译" sheetId="8" r:id="rId4"/>
-    <sheet name="Android高级应用开发-基础篇_74UI开发的2+1法则" sheetId="1" r:id="rId5"/>
-    <sheet name="版本控制" sheetId="2" r:id="rId6"/>
-    <sheet name="Adapter" sheetId="3" r:id="rId7"/>
-    <sheet name="消息机制" sheetId="6" r:id="rId8"/>
-    <sheet name="消息机制模型" sheetId="10" r:id="rId9"/>
-    <sheet name="基于监听的事件处理机制" sheetId="12" r:id="rId10"/>
-    <sheet name="==与equals" sheetId="7" r:id="rId11"/>
-    <sheet name="hashCode" sheetId="9" r:id="rId12"/>
-    <sheet name="IO" sheetId="13" r:id="rId13"/>
+    <sheet name="Android Doc reads" sheetId="16" r:id="rId1"/>
+    <sheet name="Activity_Lifecycle" sheetId="15" r:id="rId2"/>
+    <sheet name="ContentProvider" sheetId="4" r:id="rId3"/>
+    <sheet name="Android高级应用开发-深入篇" sheetId="5" r:id="rId4"/>
+    <sheet name="反编译" sheetId="8" r:id="rId5"/>
+    <sheet name="Android高级应用开发-基础篇_74UI开发的2+1法则" sheetId="1" r:id="rId6"/>
+    <sheet name="版本控制" sheetId="2" r:id="rId7"/>
+    <sheet name="Adapter" sheetId="3" r:id="rId8"/>
+    <sheet name="消息机制" sheetId="6" r:id="rId9"/>
+    <sheet name="消息机制模型" sheetId="10" r:id="rId10"/>
+    <sheet name="基于监听的事件处理机制" sheetId="12" r:id="rId11"/>
+    <sheet name="==与equals" sheetId="7" r:id="rId12"/>
+    <sheet name="hashCode" sheetId="9" r:id="rId13"/>
+    <sheet name="IO" sheetId="13" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Android高级应用开发-深入篇'!$A$1:$C$222</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Android高级应用开发-深入篇'!$A$1:$D$225</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Android高级应用开发-深入篇'!$A$1:$C$222</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Android高级应用开发-深入篇'!$A$1:$D$225</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
 </workbook>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="439">
   <si>
     <t>Activity</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1735,9 +1736,6 @@
     <t>onStop()</t>
   </si>
   <si>
-    <t>onRestart()</t>
-  </si>
-  <si>
     <t>onDestroy()</t>
   </si>
   <si>
@@ -1787,13 +1785,37 @@
   </si>
   <si>
     <t>Do What</t>
+  </si>
+  <si>
+    <t>https://developer.android.google.cn/guide/components/activities/intro-activities</t>
+  </si>
+  <si>
+    <t>Introduction to Activities</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>https://developer.android.google.cn/guide/components/activities/activity-lifecycle</t>
+  </si>
+  <si>
+    <t>Understand the Activity Lifecycle</t>
+  </si>
+  <si>
+    <t>http://android-developers.blogspot.com/2011/06/things-that-cannot-change.html</t>
+  </si>
+  <si>
+    <t>Things That Cannot Change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2059,6 +2081,14 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2618,11 +2648,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2872,6 +2903,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2929,13 +2965,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{66AFF3AD-B4DE-FA4E-AB57-26B45159E82C}"/>
   </cellStyles>
@@ -7605,139 +7638,854 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695F25B9-FD59-DD4E-A097-058E28B48012}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD58857B-D0A1-5746-959D-8AF492D5EE51}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="162" t="s">
-        <v>428</v>
-      </c>
-      <c r="B1" s="162" t="s">
-        <v>416</v>
-      </c>
-      <c r="C1" s="162" t="s">
-        <v>420</v>
-      </c>
-      <c r="D1" s="162" t="s">
-        <v>423</v>
-      </c>
-      <c r="E1" s="166" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>432</v>
+      </c>
+      <c r="B1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C1" s="167" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="163" t="s">
-        <v>411</v>
-      </c>
-      <c r="B2" s="164" t="s">
-        <v>419</v>
-      </c>
-      <c r="C2" s="164" t="s">
-        <v>419</v>
-      </c>
-      <c r="D2" s="163" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="163" t="s">
-        <v>409</v>
-      </c>
-      <c r="B3" s="163" t="s">
-        <v>417</v>
-      </c>
-      <c r="C3" s="164" t="s">
-        <v>419</v>
-      </c>
-      <c r="D3" s="163" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="163" t="s">
-        <v>410</v>
-      </c>
-      <c r="B4" s="163" t="s">
-        <v>417</v>
-      </c>
-      <c r="C4" s="163" t="s">
-        <v>421</v>
-      </c>
-      <c r="D4" s="163" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="163" t="s">
-        <v>412</v>
-      </c>
-      <c r="B5" s="165" t="s">
-        <v>418</v>
-      </c>
-      <c r="C5" s="163" t="s">
-        <v>430</v>
-      </c>
-      <c r="D5" s="163" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="163" t="s">
-        <v>413</v>
-      </c>
-      <c r="B6" s="163" t="s">
-        <v>429</v>
-      </c>
-      <c r="C6" s="164" t="s">
-        <v>419</v>
-      </c>
-      <c r="D6" s="163" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="163" t="s">
-        <v>414</v>
-      </c>
-      <c r="B7" s="164" t="s">
-        <v>419</v>
-      </c>
-      <c r="C7" s="164" t="s">
-        <v>419</v>
-      </c>
-      <c r="D7" s="164" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="163" t="s">
-        <v>415</v>
-      </c>
-      <c r="B8" s="164" t="s">
-        <v>419</v>
-      </c>
-      <c r="C8" s="164" t="s">
-        <v>419</v>
-      </c>
-      <c r="D8" s="163" t="s">
-        <v>422</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C3" s="167" t="s">
+        <v>437</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{CCE21B43-37BE-6D4F-A42F-AFF31417B473}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{A7FB048C-38FE-DE4F-BC6C-9A1FD3DD21BF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA80C652-EB11-2747-89DA-E4ABA79A811D}">
+  <dimension ref="A2:T38"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:20">
+      <c r="A2" s="94"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="94"/>
+      <c r="M2" s="94"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="94"/>
+      <c r="R2" s="94"/>
+      <c r="S2" s="94"/>
+      <c r="T2" s="94"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="94"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="94"/>
+      <c r="O3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
+      <c r="S3" s="94"/>
+      <c r="T3" s="94"/>
+    </row>
+    <row r="4" spans="1:20" ht="27" thickBot="1">
+      <c r="A4" s="94"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="119" t="s">
+        <v>388</v>
+      </c>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="94"/>
+      <c r="Q4" s="119" t="s">
+        <v>389</v>
+      </c>
+      <c r="R4" s="94"/>
+      <c r="S4" s="94"/>
+      <c r="T4" s="94"/>
+    </row>
+    <row r="5" spans="1:20" ht="16" thickBot="1">
+      <c r="A5" s="94"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="100"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="99"/>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="99"/>
+      <c r="T5" s="100"/>
+    </row>
+    <row r="6" spans="1:20" ht="21" customHeight="1">
+      <c r="A6" s="94"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="152" t="s">
+        <v>392</v>
+      </c>
+      <c r="G6" s="153"/>
+      <c r="H6" s="154"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="101"/>
+      <c r="O6" s="96"/>
+      <c r="P6" s="96"/>
+      <c r="Q6" s="96"/>
+      <c r="R6" s="96"/>
+      <c r="S6" s="96"/>
+      <c r="T6" s="102"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="94"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="156"/>
+      <c r="H7" s="157"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="94"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="101"/>
+      <c r="O7" s="96"/>
+      <c r="P7" s="96"/>
+      <c r="Q7" s="96"/>
+      <c r="R7" s="96"/>
+      <c r="S7" s="96"/>
+      <c r="T7" s="102"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="94"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="155"/>
+      <c r="G8" s="156"/>
+      <c r="H8" s="157"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="102"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
+      <c r="M8" s="94"/>
+      <c r="N8" s="101"/>
+      <c r="O8" s="96"/>
+      <c r="P8" s="96"/>
+      <c r="Q8" s="96"/>
+      <c r="R8" s="96"/>
+      <c r="S8" s="96"/>
+      <c r="T8" s="102"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="94"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="101"/>
+      <c r="F9" s="155"/>
+      <c r="G9" s="156"/>
+      <c r="H9" s="157"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
+      <c r="M9" s="94"/>
+      <c r="N9" s="101"/>
+      <c r="O9" s="93"/>
+      <c r="P9" s="93"/>
+      <c r="Q9" s="96"/>
+      <c r="R9" s="96"/>
+      <c r="S9" s="96"/>
+      <c r="T9" s="102"/>
+    </row>
+    <row r="10" spans="1:20" ht="16" thickBot="1">
+      <c r="A10" s="94"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="101"/>
+      <c r="F10" s="158"/>
+      <c r="G10" s="159"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="129"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="94"/>
+      <c r="L10" s="94"/>
+      <c r="M10" s="94"/>
+      <c r="N10" s="101"/>
+      <c r="O10" s="93"/>
+      <c r="P10" s="93"/>
+      <c r="Q10" s="96"/>
+      <c r="R10" s="96"/>
+      <c r="S10" s="96"/>
+      <c r="T10" s="102"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="94"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="101"/>
+      <c r="G11" s="129"/>
+      <c r="H11" s="96"/>
+      <c r="I11" s="96"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="94"/>
+      <c r="M11" s="94"/>
+      <c r="N11" s="101"/>
+      <c r="O11" s="93"/>
+      <c r="P11" s="93"/>
+      <c r="Q11" s="96"/>
+      <c r="R11" s="96"/>
+      <c r="S11" s="96"/>
+      <c r="T11" s="102"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="94"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="101"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="94"/>
+      <c r="L12" s="94"/>
+      <c r="M12" s="94"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="93"/>
+      <c r="P12" s="93"/>
+      <c r="Q12" s="96"/>
+      <c r="R12" s="96"/>
+      <c r="S12" s="96"/>
+      <c r="T12" s="102"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="94"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="101"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+      <c r="I13" s="96"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="101"/>
+      <c r="O13" s="93"/>
+      <c r="P13" s="93"/>
+      <c r="Q13" s="96"/>
+      <c r="R13" s="96"/>
+      <c r="S13" s="96"/>
+      <c r="T13" s="102"/>
+    </row>
+    <row r="14" spans="1:20" ht="27" thickBot="1">
+      <c r="A14" s="94"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="120" t="s">
+        <v>386</v>
+      </c>
+      <c r="H14" s="96"/>
+      <c r="I14" s="96"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="94"/>
+      <c r="L14" s="118" t="s">
+        <v>393</v>
+      </c>
+      <c r="M14" s="94"/>
+      <c r="N14" s="101"/>
+      <c r="O14" s="93"/>
+      <c r="P14" s="93"/>
+      <c r="Q14" s="123"/>
+      <c r="R14" s="96"/>
+      <c r="S14" s="96"/>
+      <c r="T14" s="102"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="94"/>
+      <c r="B15" s="94"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="101"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="109"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="109"/>
+      <c r="I15" s="110"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="94"/>
+      <c r="L15" s="94"/>
+      <c r="M15" s="94"/>
+      <c r="N15" s="101"/>
+      <c r="O15" s="96"/>
+      <c r="P15" s="96"/>
+      <c r="Q15" s="96"/>
+      <c r="R15" s="96"/>
+      <c r="S15" s="96"/>
+      <c r="T15" s="102"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="94"/>
+      <c r="B16" s="94"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="94"/>
+      <c r="L16" s="94"/>
+      <c r="M16" s="94"/>
+      <c r="N16" s="101"/>
+      <c r="O16" s="96"/>
+      <c r="P16" s="96"/>
+      <c r="Q16" s="96"/>
+      <c r="R16" s="96"/>
+      <c r="S16" s="96"/>
+      <c r="T16" s="102"/>
+    </row>
+    <row r="17" spans="1:20" ht="26">
+      <c r="A17" s="94"/>
+      <c r="B17" s="94"/>
+      <c r="C17" s="94"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="94"/>
+      <c r="L17" s="94"/>
+      <c r="M17" s="94"/>
+      <c r="N17" s="101"/>
+      <c r="O17" s="121"/>
+      <c r="P17" s="118"/>
+      <c r="Q17" s="121"/>
+      <c r="R17" s="121"/>
+      <c r="S17" s="121"/>
+      <c r="T17" s="102"/>
+    </row>
+    <row r="18" spans="1:20" ht="26">
+      <c r="A18" s="94"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="101"/>
+      <c r="E18" s="111"/>
+      <c r="H18" s="96"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="102"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="94"/>
+      <c r="N18" s="101"/>
+      <c r="O18" s="121"/>
+      <c r="P18" s="128" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q18" s="118"/>
+      <c r="R18" s="121"/>
+      <c r="S18" s="121"/>
+      <c r="T18" s="102"/>
+    </row>
+    <row r="19" spans="1:20" ht="27" thickBot="1">
+      <c r="A19" s="94"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="96"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="102"/>
+      <c r="K19" s="94"/>
+      <c r="L19" s="94"/>
+      <c r="M19" s="94"/>
+      <c r="N19" s="101"/>
+      <c r="O19" s="121"/>
+      <c r="P19" s="118"/>
+      <c r="Q19" s="121"/>
+      <c r="R19" s="121"/>
+      <c r="S19" s="121"/>
+      <c r="T19" s="102"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="94"/>
+      <c r="B20" s="94"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="124"/>
+      <c r="H20" s="96"/>
+      <c r="I20" s="112"/>
+      <c r="J20" s="102"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="94"/>
+      <c r="M20" s="94"/>
+      <c r="N20" s="101"/>
+      <c r="O20" s="96"/>
+      <c r="P20" s="96"/>
+      <c r="Q20" s="96"/>
+      <c r="R20" s="96"/>
+      <c r="S20" s="96"/>
+      <c r="T20" s="102"/>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="94"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="94"/>
+      <c r="G21" s="125"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="102"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="94"/>
+      <c r="M21" s="94"/>
+      <c r="N21" s="101"/>
+      <c r="O21" s="94"/>
+      <c r="P21" s="94"/>
+      <c r="Q21" s="96"/>
+      <c r="R21" s="96"/>
+      <c r="S21" s="96"/>
+      <c r="T21" s="102"/>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="94"/>
+      <c r="B22" s="94"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="125"/>
+      <c r="H22" s="96"/>
+      <c r="I22" s="112"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="94"/>
+      <c r="M22" s="94"/>
+      <c r="N22" s="101"/>
+      <c r="O22" s="94"/>
+      <c r="P22" s="94"/>
+      <c r="Q22" s="96"/>
+      <c r="R22" s="96"/>
+      <c r="S22" s="96"/>
+      <c r="T22" s="102"/>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="94"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="101"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="125"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="112"/>
+      <c r="J23" s="102"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="94"/>
+      <c r="M23" s="94"/>
+      <c r="N23" s="101"/>
+      <c r="O23" s="94"/>
+      <c r="P23" s="94"/>
+      <c r="Q23" s="96"/>
+      <c r="R23" s="96"/>
+      <c r="S23" s="96"/>
+      <c r="T23" s="102"/>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="94"/>
+      <c r="B24" s="94"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="96"/>
+      <c r="G24" s="125"/>
+      <c r="H24" s="96"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="102"/>
+      <c r="K24" s="94"/>
+      <c r="L24" s="94"/>
+      <c r="M24" s="94"/>
+      <c r="N24" s="101"/>
+      <c r="O24" s="96"/>
+      <c r="P24" s="96"/>
+      <c r="Q24" s="96"/>
+      <c r="R24" s="96"/>
+      <c r="S24" s="96"/>
+      <c r="T24" s="102"/>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="94"/>
+      <c r="B25" s="94"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="101"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="125"/>
+      <c r="H25" s="96"/>
+      <c r="I25" s="112"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="94"/>
+      <c r="L25" s="94"/>
+      <c r="M25" s="94"/>
+      <c r="N25" s="101"/>
+      <c r="O25" s="96"/>
+      <c r="P25" s="96"/>
+      <c r="Q25" s="96"/>
+      <c r="R25" s="96"/>
+      <c r="S25" s="96"/>
+      <c r="T25" s="102"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="94"/>
+      <c r="B26" s="94"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="96"/>
+      <c r="G26" s="126"/>
+      <c r="H26" s="96"/>
+      <c r="I26" s="112"/>
+      <c r="J26" s="102"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="94"/>
+      <c r="N26" s="101"/>
+      <c r="O26" s="96"/>
+      <c r="P26" s="96"/>
+      <c r="Q26" s="96"/>
+      <c r="R26" s="96"/>
+      <c r="S26" s="96"/>
+      <c r="T26" s="102"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="94"/>
+      <c r="B27" s="94"/>
+      <c r="C27" s="94"/>
+      <c r="D27" s="101"/>
+      <c r="E27" s="111"/>
+      <c r="F27" s="96"/>
+      <c r="G27" s="126"/>
+      <c r="H27" s="96"/>
+      <c r="I27" s="112"/>
+      <c r="J27" s="102"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="94"/>
+      <c r="N27" s="101"/>
+      <c r="O27" s="96"/>
+      <c r="P27" s="96"/>
+      <c r="Q27" s="96"/>
+      <c r="R27" s="96"/>
+      <c r="S27" s="96"/>
+      <c r="T27" s="102"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="94"/>
+      <c r="B28" s="94"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="101"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="97"/>
+      <c r="G28" s="126"/>
+      <c r="H28" s="97"/>
+      <c r="I28" s="114"/>
+      <c r="J28" s="102"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="94"/>
+      <c r="N28" s="101"/>
+      <c r="O28" s="96"/>
+      <c r="P28" s="97"/>
+      <c r="Q28" s="97"/>
+      <c r="R28" s="97"/>
+      <c r="S28" s="97"/>
+      <c r="T28" s="102"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="94"/>
+      <c r="B29" s="94"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="96"/>
+      <c r="G29" s="125" t="s">
+        <v>391</v>
+      </c>
+      <c r="H29" s="96"/>
+      <c r="I29" s="112"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
+      <c r="N29" s="101"/>
+      <c r="O29" s="96"/>
+      <c r="P29" s="96"/>
+      <c r="Q29" s="96"/>
+      <c r="R29" s="96"/>
+      <c r="S29" s="96"/>
+      <c r="T29" s="102"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="94"/>
+      <c r="B30" s="94"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="101"/>
+      <c r="E30" s="111"/>
+      <c r="F30" s="96"/>
+      <c r="G30" s="125" t="s">
+        <v>391</v>
+      </c>
+      <c r="H30" s="96"/>
+      <c r="I30" s="112"/>
+      <c r="J30" s="102"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="94"/>
+      <c r="N30" s="101"/>
+      <c r="O30" s="96"/>
+      <c r="P30" s="96"/>
+      <c r="Q30" s="96"/>
+      <c r="R30" s="96"/>
+      <c r="S30" s="96"/>
+      <c r="T30" s="102"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="D31" s="103"/>
+      <c r="E31" s="111"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="125" t="s">
+        <v>391</v>
+      </c>
+      <c r="H31" s="96"/>
+      <c r="I31" s="112"/>
+      <c r="J31" s="104"/>
+      <c r="N31" s="103"/>
+      <c r="O31" s="96"/>
+      <c r="P31" s="96"/>
+      <c r="Q31" s="96"/>
+      <c r="R31" s="96"/>
+      <c r="S31" s="96"/>
+      <c r="T31" s="102"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="C32" s="93"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="111"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="125" t="s">
+        <v>391</v>
+      </c>
+      <c r="H32" s="96"/>
+      <c r="I32" s="112"/>
+      <c r="J32" s="104"/>
+      <c r="N32" s="103"/>
+      <c r="O32" s="96"/>
+      <c r="P32" s="96"/>
+      <c r="Q32" s="96"/>
+      <c r="R32" s="96"/>
+      <c r="S32" s="96"/>
+      <c r="T32" s="102"/>
+    </row>
+    <row r="33" spans="4:20" ht="16" thickBot="1">
+      <c r="D33" s="103"/>
+      <c r="E33" s="111"/>
+      <c r="G33" s="127"/>
+      <c r="H33" s="96"/>
+      <c r="I33" s="112"/>
+      <c r="J33" s="104"/>
+      <c r="N33" s="103"/>
+      <c r="O33" s="96"/>
+      <c r="P33" s="96"/>
+      <c r="Q33" s="96"/>
+      <c r="R33" s="96"/>
+      <c r="S33" s="96"/>
+      <c r="T33" s="102"/>
+    </row>
+    <row r="34" spans="4:20" ht="26">
+      <c r="D34" s="103"/>
+      <c r="E34" s="111"/>
+      <c r="F34" s="122" t="s">
+        <v>387</v>
+      </c>
+      <c r="G34" s="96"/>
+      <c r="H34" s="96"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="104"/>
+      <c r="N34" s="103"/>
+      <c r="O34" s="96"/>
+      <c r="P34" s="96"/>
+      <c r="Q34" s="96"/>
+      <c r="R34" s="96"/>
+      <c r="S34" s="96"/>
+      <c r="T34" s="102"/>
+    </row>
+    <row r="35" spans="4:20">
+      <c r="D35" s="103"/>
+      <c r="E35" s="111"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="96"/>
+      <c r="I35" s="112"/>
+      <c r="J35" s="104"/>
+      <c r="N35" s="103"/>
+      <c r="O35" s="96"/>
+      <c r="P35" s="96"/>
+      <c r="Q35" s="96"/>
+      <c r="R35" s="96"/>
+      <c r="S35" s="96"/>
+      <c r="T35" s="102"/>
+    </row>
+    <row r="36" spans="4:20">
+      <c r="D36" s="103"/>
+      <c r="E36" s="111"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="96"/>
+      <c r="H36" s="96"/>
+      <c r="I36" s="112"/>
+      <c r="J36" s="104"/>
+      <c r="N36" s="103"/>
+      <c r="O36" s="96"/>
+      <c r="P36" s="96"/>
+      <c r="Q36" s="96"/>
+      <c r="R36" s="96"/>
+      <c r="S36" s="96"/>
+      <c r="T36" s="102"/>
+    </row>
+    <row r="37" spans="4:20" ht="16" thickBot="1">
+      <c r="D37" s="103"/>
+      <c r="E37" s="115"/>
+      <c r="F37" s="116"/>
+      <c r="G37" s="116"/>
+      <c r="H37" s="116"/>
+      <c r="I37" s="117"/>
+      <c r="J37" s="104"/>
+      <c r="N37" s="103"/>
+      <c r="O37" s="96"/>
+      <c r="P37" s="96"/>
+      <c r="Q37" s="96"/>
+      <c r="R37" s="96"/>
+      <c r="S37" s="96"/>
+      <c r="T37" s="102"/>
+    </row>
+    <row r="38" spans="4:20" ht="16" thickBot="1">
+      <c r="D38" s="105"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="106"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="107"/>
+      <c r="N38" s="105"/>
+      <c r="O38" s="106"/>
+      <c r="P38" s="106"/>
+      <c r="Q38" s="106"/>
+      <c r="R38" s="106"/>
+      <c r="S38" s="106"/>
+      <c r="T38" s="107"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F6:H10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7778B8-D430-A34A-995E-0F83AC473C52}">
   <dimension ref="E8:K35"/>
   <sheetViews>
@@ -7817,16 +8565,16 @@
     </row>
     <row r="18" spans="5:8">
       <c r="E18" s="137"/>
-      <c r="F18" s="156" t="s">
+      <c r="F18" s="161" t="s">
         <v>395</v>
       </c>
-      <c r="G18" s="157"/>
+      <c r="G18" s="162"/>
       <c r="H18" s="135"/>
     </row>
     <row r="19" spans="5:8">
       <c r="E19" s="137"/>
-      <c r="F19" s="158"/>
-      <c r="G19" s="159"/>
+      <c r="F19" s="163"/>
+      <c r="G19" s="164"/>
       <c r="H19" s="135"/>
     </row>
     <row r="20" spans="5:8">
@@ -7922,7 +8670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:K25"/>
   <sheetViews>
@@ -8137,7 +8885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A3:E21"/>
   <sheetViews>
@@ -8320,7 +9068,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE8B8C4-352E-054D-A843-45DFD254B784}">
   <dimension ref="B2:J61"/>
   <sheetViews>
@@ -8341,10 +9089,10 @@
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="H12" s="160" t="s">
+      <c r="H12" s="165" t="s">
         <v>399</v>
       </c>
-      <c r="I12" s="160"/>
+      <c r="I12" s="165"/>
     </row>
     <row r="14" spans="2:10">
       <c r="J14" t="s">
@@ -8357,10 +9105,10 @@
       </c>
     </row>
     <row r="28" spans="2:9">
-      <c r="H28" s="161" t="s">
+      <c r="H28" s="166" t="s">
         <v>403</v>
       </c>
-      <c r="I28" s="161"/>
+      <c r="I28" s="166"/>
     </row>
     <row r="39" spans="2:9">
       <c r="B39" t="s">
@@ -8368,10 +9116,10 @@
       </c>
     </row>
     <row r="43" spans="2:9">
-      <c r="H43" s="160" t="s">
+      <c r="H43" s="165" t="s">
         <v>406</v>
       </c>
-      <c r="I43" s="160"/>
+      <c r="I43" s="165"/>
     </row>
     <row r="54" spans="2:9">
       <c r="B54" t="s">
@@ -8379,10 +9127,10 @@
       </c>
     </row>
     <row r="59" spans="2:9">
-      <c r="H59" s="161" t="s">
+      <c r="H59" s="166" t="s">
         <v>403</v>
       </c>
-      <c r="I59" s="161"/>
+      <c r="I59" s="166"/>
     </row>
     <row r="61" spans="2:9">
       <c r="G61" t="s">
@@ -8402,6 +9150,125 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695F25B9-FD59-DD4E-A097-058E28B48012}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="143" t="s">
+        <v>427</v>
+      </c>
+      <c r="B1" s="143" t="s">
+        <v>415</v>
+      </c>
+      <c r="C1" s="143" t="s">
+        <v>419</v>
+      </c>
+      <c r="D1" s="143" t="s">
+        <v>422</v>
+      </c>
+      <c r="E1" s="147" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="144" t="s">
+        <v>411</v>
+      </c>
+      <c r="B2" s="145" t="s">
+        <v>418</v>
+      </c>
+      <c r="C2" s="145" t="s">
+        <v>418</v>
+      </c>
+      <c r="D2" s="144" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="144" t="s">
+        <v>409</v>
+      </c>
+      <c r="B3" s="144" t="s">
+        <v>416</v>
+      </c>
+      <c r="C3" s="145" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3" s="144" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="144" t="s">
+        <v>410</v>
+      </c>
+      <c r="B4" s="144" t="s">
+        <v>416</v>
+      </c>
+      <c r="C4" s="144" t="s">
+        <v>420</v>
+      </c>
+      <c r="D4" s="144" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="144" t="s">
+        <v>412</v>
+      </c>
+      <c r="B5" s="146" t="s">
+        <v>417</v>
+      </c>
+      <c r="C5" s="144" t="s">
+        <v>429</v>
+      </c>
+      <c r="D5" s="144" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="144" t="s">
+        <v>413</v>
+      </c>
+      <c r="B6" s="144" t="s">
+        <v>428</v>
+      </c>
+      <c r="C6" s="145" t="s">
+        <v>418</v>
+      </c>
+      <c r="D6" s="144" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="144" t="s">
+        <v>414</v>
+      </c>
+      <c r="B7" s="145" t="s">
+        <v>418</v>
+      </c>
+      <c r="C7" s="145" t="s">
+        <v>418</v>
+      </c>
+      <c r="D7" s="144" t="s">
+        <v>421</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:Q30"/>
   <sheetViews>
@@ -8817,7 +9684,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D224"/>
@@ -10798,7 +11665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:I20"/>
   <sheetViews>
@@ -10912,7 +11779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:Q39"/>
   <sheetViews>
@@ -11243,7 +12110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:G13"/>
   <sheetViews>
@@ -11299,7 +12166,7 @@
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="148" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -11319,7 +12186,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="143"/>
+      <c r="B6" s="148"/>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
@@ -11335,7 +12202,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="143"/>
+      <c r="B7" s="148"/>
       <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
@@ -11353,7 +12220,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="143"/>
+      <c r="B8" s="148"/>
       <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
@@ -11371,7 +12238,7 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="143"/>
+      <c r="B9" s="148"/>
       <c r="C9" s="16" t="s">
         <v>33</v>
       </c>
@@ -11389,7 +12256,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="26">
-      <c r="B10" s="143"/>
+      <c r="B10" s="148"/>
       <c r="C10" s="16" t="s">
         <v>13</v>
       </c>
@@ -11407,7 +12274,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="39">
-      <c r="B11" s="144" t="s">
+      <c r="B11" s="149" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -11427,7 +12294,7 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="145"/>
+      <c r="B12" s="150"/>
       <c r="C12" s="15" t="s">
         <v>15</v>
       </c>
@@ -11441,7 +12308,7 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="146"/>
+      <c r="B13" s="151"/>
       <c r="C13" s="15" t="s">
         <v>16</v>
       </c>
@@ -11467,7 +12334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:N24"/>
   <sheetViews>
@@ -11627,7 +12494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:U32"/>
   <sheetViews>
@@ -11886,795 +12753,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA80C652-EB11-2747-89DA-E4ABA79A811D}">
-  <dimension ref="A2:T38"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:20">
-      <c r="A2" s="94"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
-      <c r="G2" s="94"/>
-      <c r="H2" s="94"/>
-      <c r="I2" s="94"/>
-      <c r="J2" s="94"/>
-      <c r="K2" s="94"/>
-      <c r="L2" s="94"/>
-      <c r="M2" s="94"/>
-      <c r="N2" s="94"/>
-      <c r="O2" s="94"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="94"/>
-      <c r="R2" s="94"/>
-      <c r="S2" s="94"/>
-      <c r="T2" s="94"/>
-    </row>
-    <row r="3" spans="1:20">
-      <c r="A3" s="94"/>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
-      <c r="Q3" s="94"/>
-      <c r="R3" s="94"/>
-      <c r="S3" s="94"/>
-      <c r="T3" s="94"/>
-    </row>
-    <row r="4" spans="1:20" ht="27" thickBot="1">
-      <c r="A4" s="94"/>
-      <c r="B4" s="94"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="119" t="s">
-        <v>388</v>
-      </c>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="119" t="s">
-        <v>389</v>
-      </c>
-      <c r="R4" s="94"/>
-      <c r="S4" s="94"/>
-      <c r="T4" s="94"/>
-    </row>
-    <row r="5" spans="1:20" ht="16" thickBot="1">
-      <c r="A5" s="94"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="98"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="99"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="94"/>
-      <c r="M5" s="94"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="99"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="99"/>
-      <c r="R5" s="99"/>
-      <c r="S5" s="99"/>
-      <c r="T5" s="100"/>
-    </row>
-    <row r="6" spans="1:20" ht="21" customHeight="1">
-      <c r="A6" s="94"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="147" t="s">
-        <v>392</v>
-      </c>
-      <c r="G6" s="148"/>
-      <c r="H6" s="149"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="94"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="96"/>
-      <c r="P6" s="96"/>
-      <c r="Q6" s="96"/>
-      <c r="R6" s="96"/>
-      <c r="S6" s="96"/>
-      <c r="T6" s="102"/>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="94"/>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="150"/>
-      <c r="G7" s="151"/>
-      <c r="H7" s="152"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="102"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="101"/>
-      <c r="O7" s="96"/>
-      <c r="P7" s="96"/>
-      <c r="Q7" s="96"/>
-      <c r="R7" s="96"/>
-      <c r="S7" s="96"/>
-      <c r="T7" s="102"/>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="94"/>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="96"/>
-      <c r="F8" s="150"/>
-      <c r="G8" s="151"/>
-      <c r="H8" s="152"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="102"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
-      <c r="M8" s="94"/>
-      <c r="N8" s="101"/>
-      <c r="O8" s="96"/>
-      <c r="P8" s="96"/>
-      <c r="Q8" s="96"/>
-      <c r="R8" s="96"/>
-      <c r="S8" s="96"/>
-      <c r="T8" s="102"/>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="94"/>
-      <c r="B9" s="94"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="101"/>
-      <c r="F9" s="150"/>
-      <c r="G9" s="151"/>
-      <c r="H9" s="152"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="102"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="93"/>
-      <c r="P9" s="93"/>
-      <c r="Q9" s="96"/>
-      <c r="R9" s="96"/>
-      <c r="S9" s="96"/>
-      <c r="T9" s="102"/>
-    </row>
-    <row r="10" spans="1:20" ht="16" thickBot="1">
-      <c r="A10" s="94"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="101"/>
-      <c r="F10" s="153"/>
-      <c r="G10" s="154"/>
-      <c r="H10" s="155"/>
-      <c r="I10" s="129"/>
-      <c r="J10" s="102"/>
-      <c r="K10" s="94"/>
-      <c r="L10" s="94"/>
-      <c r="M10" s="94"/>
-      <c r="N10" s="101"/>
-      <c r="O10" s="93"/>
-      <c r="P10" s="93"/>
-      <c r="Q10" s="96"/>
-      <c r="R10" s="96"/>
-      <c r="S10" s="96"/>
-      <c r="T10" s="102"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="94"/>
-      <c r="B11" s="94"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="101"/>
-      <c r="G11" s="129"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="96"/>
-      <c r="J11" s="102"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="101"/>
-      <c r="O11" s="93"/>
-      <c r="P11" s="93"/>
-      <c r="Q11" s="96"/>
-      <c r="R11" s="96"/>
-      <c r="S11" s="96"/>
-      <c r="T11" s="102"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="94"/>
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="101"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="96"/>
-      <c r="I12" s="96"/>
-      <c r="J12" s="102"/>
-      <c r="K12" s="94"/>
-      <c r="L12" s="94"/>
-      <c r="M12" s="94"/>
-      <c r="N12" s="101"/>
-      <c r="O12" s="93"/>
-      <c r="P12" s="93"/>
-      <c r="Q12" s="96"/>
-      <c r="R12" s="96"/>
-      <c r="S12" s="96"/>
-      <c r="T12" s="102"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="94"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="101"/>
-      <c r="G13" s="96"/>
-      <c r="H13" s="96"/>
-      <c r="I13" s="96"/>
-      <c r="J13" s="102"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="94"/>
-      <c r="N13" s="101"/>
-      <c r="O13" s="93"/>
-      <c r="P13" s="93"/>
-      <c r="Q13" s="96"/>
-      <c r="R13" s="96"/>
-      <c r="S13" s="96"/>
-      <c r="T13" s="102"/>
-    </row>
-    <row r="14" spans="1:20" ht="27" thickBot="1">
-      <c r="A14" s="94"/>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="120" t="s">
-        <v>386</v>
-      </c>
-      <c r="H14" s="96"/>
-      <c r="I14" s="96"/>
-      <c r="J14" s="102"/>
-      <c r="K14" s="94"/>
-      <c r="L14" s="118" t="s">
-        <v>393</v>
-      </c>
-      <c r="M14" s="94"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="93"/>
-      <c r="P14" s="93"/>
-      <c r="Q14" s="123"/>
-      <c r="R14" s="96"/>
-      <c r="S14" s="96"/>
-      <c r="T14" s="102"/>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="94"/>
-      <c r="B15" s="94"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="101"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="109"/>
-      <c r="H15" s="109"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="102"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="M15" s="94"/>
-      <c r="N15" s="101"/>
-      <c r="O15" s="96"/>
-      <c r="P15" s="96"/>
-      <c r="Q15" s="96"/>
-      <c r="R15" s="96"/>
-      <c r="S15" s="96"/>
-      <c r="T15" s="102"/>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="94"/>
-      <c r="B16" s="94"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="112"/>
-      <c r="J16" s="102"/>
-      <c r="K16" s="94"/>
-      <c r="L16" s="94"/>
-      <c r="M16" s="94"/>
-      <c r="N16" s="101"/>
-      <c r="O16" s="96"/>
-      <c r="P16" s="96"/>
-      <c r="Q16" s="96"/>
-      <c r="R16" s="96"/>
-      <c r="S16" s="96"/>
-      <c r="T16" s="102"/>
-    </row>
-    <row r="17" spans="1:20" ht="26">
-      <c r="A17" s="94"/>
-      <c r="B17" s="94"/>
-      <c r="C17" s="94"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="102"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="M17" s="94"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="121"/>
-      <c r="P17" s="118"/>
-      <c r="Q17" s="121"/>
-      <c r="R17" s="121"/>
-      <c r="S17" s="121"/>
-      <c r="T17" s="102"/>
-    </row>
-    <row r="18" spans="1:20" ht="26">
-      <c r="A18" s="94"/>
-      <c r="B18" s="94"/>
-      <c r="C18" s="94"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="111"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="112"/>
-      <c r="J18" s="102"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="94"/>
-      <c r="N18" s="101"/>
-      <c r="O18" s="121"/>
-      <c r="P18" s="128" t="s">
-        <v>390</v>
-      </c>
-      <c r="Q18" s="118"/>
-      <c r="R18" s="121"/>
-      <c r="S18" s="121"/>
-      <c r="T18" s="102"/>
-    </row>
-    <row r="19" spans="1:20" ht="27" thickBot="1">
-      <c r="A19" s="94"/>
-      <c r="B19" s="94"/>
-      <c r="C19" s="94"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="94"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="102"/>
-      <c r="K19" s="94"/>
-      <c r="L19" s="94"/>
-      <c r="M19" s="94"/>
-      <c r="N19" s="101"/>
-      <c r="O19" s="121"/>
-      <c r="P19" s="118"/>
-      <c r="Q19" s="121"/>
-      <c r="R19" s="121"/>
-      <c r="S19" s="121"/>
-      <c r="T19" s="102"/>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20" s="94"/>
-      <c r="B20" s="94"/>
-      <c r="C20" s="94"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="96"/>
-      <c r="G20" s="124"/>
-      <c r="H20" s="96"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="102"/>
-      <c r="K20" s="94"/>
-      <c r="L20" s="94"/>
-      <c r="M20" s="94"/>
-      <c r="N20" s="101"/>
-      <c r="O20" s="96"/>
-      <c r="P20" s="96"/>
-      <c r="Q20" s="96"/>
-      <c r="R20" s="96"/>
-      <c r="S20" s="96"/>
-      <c r="T20" s="102"/>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" s="94"/>
-      <c r="B21" s="94"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="94"/>
-      <c r="G21" s="125"/>
-      <c r="H21" s="96"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="102"/>
-      <c r="K21" s="94"/>
-      <c r="L21" s="94"/>
-      <c r="M21" s="94"/>
-      <c r="N21" s="101"/>
-      <c r="O21" s="94"/>
-      <c r="P21" s="94"/>
-      <c r="Q21" s="96"/>
-      <c r="R21" s="96"/>
-      <c r="S21" s="96"/>
-      <c r="T21" s="102"/>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" s="94"/>
-      <c r="B22" s="94"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="125"/>
-      <c r="H22" s="96"/>
-      <c r="I22" s="112"/>
-      <c r="J22" s="102"/>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="101"/>
-      <c r="O22" s="94"/>
-      <c r="P22" s="94"/>
-      <c r="Q22" s="96"/>
-      <c r="R22" s="96"/>
-      <c r="S22" s="96"/>
-      <c r="T22" s="102"/>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="94"/>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="125"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="112"/>
-      <c r="J23" s="102"/>
-      <c r="K23" s="94"/>
-      <c r="L23" s="94"/>
-      <c r="M23" s="94"/>
-      <c r="N23" s="101"/>
-      <c r="O23" s="94"/>
-      <c r="P23" s="94"/>
-      <c r="Q23" s="96"/>
-      <c r="R23" s="96"/>
-      <c r="S23" s="96"/>
-      <c r="T23" s="102"/>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="94"/>
-      <c r="B24" s="94"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="111"/>
-      <c r="F24" s="96"/>
-      <c r="G24" s="125"/>
-      <c r="H24" s="96"/>
-      <c r="I24" s="112"/>
-      <c r="J24" s="102"/>
-      <c r="K24" s="94"/>
-      <c r="L24" s="94"/>
-      <c r="M24" s="94"/>
-      <c r="N24" s="101"/>
-      <c r="O24" s="96"/>
-      <c r="P24" s="96"/>
-      <c r="Q24" s="96"/>
-      <c r="R24" s="96"/>
-      <c r="S24" s="96"/>
-      <c r="T24" s="102"/>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="A25" s="94"/>
-      <c r="B25" s="94"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="111"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="125"/>
-      <c r="H25" s="96"/>
-      <c r="I25" s="112"/>
-      <c r="J25" s="102"/>
-      <c r="K25" s="94"/>
-      <c r="L25" s="94"/>
-      <c r="M25" s="94"/>
-      <c r="N25" s="101"/>
-      <c r="O25" s="96"/>
-      <c r="P25" s="96"/>
-      <c r="Q25" s="96"/>
-      <c r="R25" s="96"/>
-      <c r="S25" s="96"/>
-      <c r="T25" s="102"/>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="94"/>
-      <c r="B26" s="94"/>
-      <c r="C26" s="94"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="111"/>
-      <c r="F26" s="96"/>
-      <c r="G26" s="126"/>
-      <c r="H26" s="96"/>
-      <c r="I26" s="112"/>
-      <c r="J26" s="102"/>
-      <c r="K26" s="94"/>
-      <c r="L26" s="94"/>
-      <c r="N26" s="101"/>
-      <c r="O26" s="96"/>
-      <c r="P26" s="96"/>
-      <c r="Q26" s="96"/>
-      <c r="R26" s="96"/>
-      <c r="S26" s="96"/>
-      <c r="T26" s="102"/>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="A27" s="94"/>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="101"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="96"/>
-      <c r="G27" s="126"/>
-      <c r="H27" s="96"/>
-      <c r="I27" s="112"/>
-      <c r="J27" s="102"/>
-      <c r="K27" s="94"/>
-      <c r="L27" s="94"/>
-      <c r="N27" s="101"/>
-      <c r="O27" s="96"/>
-      <c r="P27" s="96"/>
-      <c r="Q27" s="96"/>
-      <c r="R27" s="96"/>
-      <c r="S27" s="96"/>
-      <c r="T27" s="102"/>
-    </row>
-    <row r="28" spans="1:20">
-      <c r="A28" s="94"/>
-      <c r="B28" s="94"/>
-      <c r="C28" s="94"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="111"/>
-      <c r="F28" s="97"/>
-      <c r="G28" s="126"/>
-      <c r="H28" s="97"/>
-      <c r="I28" s="114"/>
-      <c r="J28" s="102"/>
-      <c r="K28" s="94"/>
-      <c r="L28" s="94"/>
-      <c r="N28" s="101"/>
-      <c r="O28" s="96"/>
-      <c r="P28" s="97"/>
-      <c r="Q28" s="97"/>
-      <c r="R28" s="97"/>
-      <c r="S28" s="97"/>
-      <c r="T28" s="102"/>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="94"/>
-      <c r="B29" s="94"/>
-      <c r="C29" s="94"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="111"/>
-      <c r="F29" s="96"/>
-      <c r="G29" s="125" t="s">
-        <v>391</v>
-      </c>
-      <c r="H29" s="96"/>
-      <c r="I29" s="112"/>
-      <c r="J29" s="102"/>
-      <c r="K29" s="94"/>
-      <c r="L29" s="94"/>
-      <c r="N29" s="101"/>
-      <c r="O29" s="96"/>
-      <c r="P29" s="96"/>
-      <c r="Q29" s="96"/>
-      <c r="R29" s="96"/>
-      <c r="S29" s="96"/>
-      <c r="T29" s="102"/>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="94"/>
-      <c r="B30" s="94"/>
-      <c r="C30" s="94"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="111"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="125" t="s">
-        <v>391</v>
-      </c>
-      <c r="H30" s="96"/>
-      <c r="I30" s="112"/>
-      <c r="J30" s="102"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="94"/>
-      <c r="N30" s="101"/>
-      <c r="O30" s="96"/>
-      <c r="P30" s="96"/>
-      <c r="Q30" s="96"/>
-      <c r="R30" s="96"/>
-      <c r="S30" s="96"/>
-      <c r="T30" s="102"/>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="D31" s="103"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="125" t="s">
-        <v>391</v>
-      </c>
-      <c r="H31" s="96"/>
-      <c r="I31" s="112"/>
-      <c r="J31" s="104"/>
-      <c r="N31" s="103"/>
-      <c r="O31" s="96"/>
-      <c r="P31" s="96"/>
-      <c r="Q31" s="96"/>
-      <c r="R31" s="96"/>
-      <c r="S31" s="96"/>
-      <c r="T31" s="102"/>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="C32" s="93"/>
-      <c r="D32" s="103"/>
-      <c r="E32" s="111"/>
-      <c r="F32" s="96"/>
-      <c r="G32" s="125" t="s">
-        <v>391</v>
-      </c>
-      <c r="H32" s="96"/>
-      <c r="I32" s="112"/>
-      <c r="J32" s="104"/>
-      <c r="N32" s="103"/>
-      <c r="O32" s="96"/>
-      <c r="P32" s="96"/>
-      <c r="Q32" s="96"/>
-      <c r="R32" s="96"/>
-      <c r="S32" s="96"/>
-      <c r="T32" s="102"/>
-    </row>
-    <row r="33" spans="4:20" ht="16" thickBot="1">
-      <c r="D33" s="103"/>
-      <c r="E33" s="111"/>
-      <c r="G33" s="127"/>
-      <c r="H33" s="96"/>
-      <c r="I33" s="112"/>
-      <c r="J33" s="104"/>
-      <c r="N33" s="103"/>
-      <c r="O33" s="96"/>
-      <c r="P33" s="96"/>
-      <c r="Q33" s="96"/>
-      <c r="R33" s="96"/>
-      <c r="S33" s="96"/>
-      <c r="T33" s="102"/>
-    </row>
-    <row r="34" spans="4:20" ht="26">
-      <c r="D34" s="103"/>
-      <c r="E34" s="111"/>
-      <c r="F34" s="122" t="s">
-        <v>387</v>
-      </c>
-      <c r="G34" s="96"/>
-      <c r="H34" s="96"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="104"/>
-      <c r="N34" s="103"/>
-      <c r="O34" s="96"/>
-      <c r="P34" s="96"/>
-      <c r="Q34" s="96"/>
-      <c r="R34" s="96"/>
-      <c r="S34" s="96"/>
-      <c r="T34" s="102"/>
-    </row>
-    <row r="35" spans="4:20">
-      <c r="D35" s="103"/>
-      <c r="E35" s="111"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="96"/>
-      <c r="I35" s="112"/>
-      <c r="J35" s="104"/>
-      <c r="N35" s="103"/>
-      <c r="O35" s="96"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="96"/>
-      <c r="R35" s="96"/>
-      <c r="S35" s="96"/>
-      <c r="T35" s="102"/>
-    </row>
-    <row r="36" spans="4:20">
-      <c r="D36" s="103"/>
-      <c r="E36" s="111"/>
-      <c r="F36" s="96"/>
-      <c r="G36" s="96"/>
-      <c r="H36" s="96"/>
-      <c r="I36" s="112"/>
-      <c r="J36" s="104"/>
-      <c r="N36" s="103"/>
-      <c r="O36" s="96"/>
-      <c r="P36" s="96"/>
-      <c r="Q36" s="96"/>
-      <c r="R36" s="96"/>
-      <c r="S36" s="96"/>
-      <c r="T36" s="102"/>
-    </row>
-    <row r="37" spans="4:20" ht="16" thickBot="1">
-      <c r="D37" s="103"/>
-      <c r="E37" s="115"/>
-      <c r="F37" s="116"/>
-      <c r="G37" s="116"/>
-      <c r="H37" s="116"/>
-      <c r="I37" s="117"/>
-      <c r="J37" s="104"/>
-      <c r="N37" s="103"/>
-      <c r="O37" s="96"/>
-      <c r="P37" s="96"/>
-      <c r="Q37" s="96"/>
-      <c r="R37" s="96"/>
-      <c r="S37" s="96"/>
-      <c r="T37" s="102"/>
-    </row>
-    <row r="38" spans="4:20" ht="16" thickBot="1">
-      <c r="D38" s="105"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="106"/>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="107"/>
-      <c r="N38" s="105"/>
-      <c r="O38" s="106"/>
-      <c r="P38" s="106"/>
-      <c r="Q38" s="106"/>
-      <c r="R38" s="106"/>
-      <c r="S38" s="106"/>
-      <c r="T38" s="107"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F6:H10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
mesuare rendering time for vector drawable
</commit_message>
<xml_diff>
--- a/doc/android.xlsx
+++ b/doc/android.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11014"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89DB3FC-01A8-E848-89D3-448B312EF657}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0BC7D5-8F13-0F42-9582-247A51A3BE95}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Android Doc reads" sheetId="16" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="基于监听的事件处理机制" sheetId="12" r:id="rId11"/>
     <sheet name="==与equals" sheetId="7" r:id="rId12"/>
     <sheet name="hashCode" sheetId="9" r:id="rId13"/>
-    <sheet name="drawable_3" sheetId="19" r:id="rId14"/>
-    <sheet name="drawable_2" sheetId="18" r:id="rId15"/>
-    <sheet name="drawable" sheetId="17" r:id="rId16"/>
-    <sheet name="IO" sheetId="13" r:id="rId17"/>
+    <sheet name="drawabe_svg" sheetId="20" r:id="rId14"/>
+    <sheet name="drawable_分辨率" sheetId="19" r:id="rId15"/>
+    <sheet name="drawable_2" sheetId="18" r:id="rId16"/>
+    <sheet name="drawable_缩放" sheetId="17" r:id="rId17"/>
+    <sheet name="IO" sheetId="13" r:id="rId18"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Android高级应用开发-深入篇'!$A$1:$C$222</definedName>
@@ -98,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="514">
   <si>
     <t>Activity</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2012,6 +2013,33 @@
   </si>
   <si>
     <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t>1440 x 1960px</t>
+  </si>
+  <si>
+    <t>screen</t>
+  </si>
+  <si>
+    <t>ImageView</t>
+  </si>
+  <si>
+    <t>1440 x 1960 px</t>
+  </si>
+  <si>
+    <t>800 x 800 px</t>
+  </si>
+  <si>
+    <t>svg</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>16.60ms</t>
+  </si>
+  <si>
+    <t>0.18ms</t>
   </si>
 </sst>
 </file>
@@ -2980,7 +3008,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3249,12 +3277,43 @@
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="49" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3315,40 +3374,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="54" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -8930,11 +8967,11 @@
       <c r="C6" s="94"/>
       <c r="D6" s="101"/>
       <c r="E6" s="96"/>
-      <c r="F6" s="161" t="s">
+      <c r="F6" s="176" t="s">
         <v>392</v>
       </c>
-      <c r="G6" s="162"/>
-      <c r="H6" s="163"/>
+      <c r="G6" s="177"/>
+      <c r="H6" s="178"/>
       <c r="I6" s="96"/>
       <c r="J6" s="102"/>
       <c r="K6" s="94"/>
@@ -8954,9 +8991,9 @@
       <c r="C7" s="94"/>
       <c r="D7" s="101"/>
       <c r="E7" s="96"/>
-      <c r="F7" s="164"/>
-      <c r="G7" s="165"/>
-      <c r="H7" s="166"/>
+      <c r="F7" s="179"/>
+      <c r="G7" s="180"/>
+      <c r="H7" s="181"/>
       <c r="I7" s="96"/>
       <c r="J7" s="102"/>
       <c r="K7" s="95"/>
@@ -8976,9 +9013,9 @@
       <c r="C8" s="94"/>
       <c r="D8" s="101"/>
       <c r="E8" s="96"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="165"/>
-      <c r="H8" s="166"/>
+      <c r="F8" s="179"/>
+      <c r="G8" s="180"/>
+      <c r="H8" s="181"/>
       <c r="I8" s="96"/>
       <c r="J8" s="102"/>
       <c r="K8" s="94"/>
@@ -8997,9 +9034,9 @@
       <c r="B9" s="94"/>
       <c r="C9" s="94"/>
       <c r="D9" s="101"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="165"/>
-      <c r="H9" s="166"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="180"/>
+      <c r="H9" s="181"/>
       <c r="I9" s="96"/>
       <c r="J9" s="102"/>
       <c r="K9" s="94"/>
@@ -9018,9 +9055,9 @@
       <c r="B10" s="94"/>
       <c r="C10" s="94"/>
       <c r="D10" s="101"/>
-      <c r="F10" s="167"/>
-      <c r="G10" s="168"/>
-      <c r="H10" s="169"/>
+      <c r="F10" s="182"/>
+      <c r="G10" s="183"/>
+      <c r="H10" s="184"/>
       <c r="I10" s="129"/>
       <c r="J10" s="102"/>
       <c r="K10" s="94"/>
@@ -9692,16 +9729,16 @@
     </row>
     <row r="18" spans="5:8">
       <c r="E18" s="137"/>
-      <c r="F18" s="170" t="s">
+      <c r="F18" s="185" t="s">
         <v>395</v>
       </c>
-      <c r="G18" s="171"/>
+      <c r="G18" s="186"/>
       <c r="H18" s="135"/>
     </row>
     <row r="19" spans="5:8">
       <c r="E19" s="137"/>
-      <c r="F19" s="172"/>
-      <c r="G19" s="173"/>
+      <c r="F19" s="187"/>
+      <c r="G19" s="188"/>
       <c r="H19" s="135"/>
     </row>
     <row r="20" spans="5:8">
@@ -10196,11 +10233,68 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFDE749-2C0C-C548-8C4F-6EF43EA89AA0}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B1" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>507</v>
+      </c>
+      <c r="B2" t="s">
+        <v>510</v>
+      </c>
+      <c r="C2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>508</v>
+      </c>
+      <c r="B3" t="s">
+        <v>512</v>
+      </c>
+      <c r="C3" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B4">
+        <v>3.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86ED6A2-BD47-244B-AD18-088367512271}">
   <dimension ref="B2:M10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+      <selection activeCell="AY40" sqref="AY40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="15"/>
@@ -10231,8 +10325,8 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5" s="186"/>
-      <c r="G5" s="187"/>
+      <c r="F5" s="165"/>
+      <c r="G5" s="166"/>
       <c r="H5" s="19"/>
       <c r="I5" s="21"/>
       <c r="J5" s="19"/>
@@ -10241,8 +10335,8 @@
       <c r="M5" s="21"/>
     </row>
     <row r="6" spans="2:13">
-      <c r="F6" s="188"/>
-      <c r="G6" s="189"/>
+      <c r="F6" s="167"/>
+      <c r="G6" s="168"/>
       <c r="H6" s="22"/>
       <c r="I6" s="24"/>
       <c r="J6" s="22"/>
@@ -10251,8 +10345,8 @@
       <c r="M6" s="24"/>
     </row>
     <row r="7" spans="2:13" ht="16" thickBot="1">
-      <c r="F7" s="190"/>
-      <c r="G7" s="191"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="170"/>
       <c r="H7" s="25"/>
       <c r="I7" s="27"/>
       <c r="J7" s="25"/>
@@ -10299,22 +10393,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A51D4780-106D-3C46-B51D-1FAF5E0D4E2A}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="155" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="155" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="154" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20" style="35" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="155"/>
-    <col min="7" max="7" width="13.1640625" style="155" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="154"/>
+    <col min="7" max="7" width="13.1640625" style="154" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -10327,13 +10421,13 @@
       <c r="B1" s="151" t="s">
         <v>459</v>
       </c>
-      <c r="C1" s="154" t="s">
+      <c r="C1" s="191" t="s">
         <v>476</v>
       </c>
       <c r="D1" s="151" t="s">
         <v>469</v>
       </c>
-      <c r="E1" s="179" t="s">
+      <c r="E1" s="158" t="s">
         <v>493</v>
       </c>
       <c r="F1" s="151" t="s">
@@ -10350,7 +10444,7 @@
       <c r="B2" s="150" t="s">
         <v>460</v>
       </c>
-      <c r="C2" s="150" t="s">
+      <c r="C2" s="192" t="s">
         <v>470</v>
       </c>
       <c r="D2" s="150">
@@ -10359,22 +10453,22 @@
       <c r="E2" s="150">
         <v>7.91</v>
       </c>
-      <c r="F2" s="180" t="s">
+      <c r="F2" s="159" t="s">
         <v>484</v>
       </c>
-      <c r="G2" s="180" t="s">
+      <c r="G2" s="159" t="s">
         <v>485</v>
       </c>
-      <c r="K2" s="155"/>
+      <c r="K2" s="154"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="150" t="s">
         <v>487</v>
       </c>
-      <c r="B3" s="182" t="s">
+      <c r="B3" s="161" t="s">
         <v>461</v>
       </c>
-      <c r="C3" s="150" t="s">
+      <c r="C3" s="192" t="s">
         <v>471</v>
       </c>
       <c r="D3" s="150">
@@ -10383,13 +10477,13 @@
       <c r="E3" s="150">
         <v>4.45</v>
       </c>
-      <c r="F3" s="180" t="s">
+      <c r="F3" s="159" t="s">
         <v>483</v>
       </c>
-      <c r="G3" s="180" t="s">
+      <c r="G3" s="159" t="s">
         <v>483</v>
       </c>
-      <c r="K3" s="155"/>
+      <c r="K3" s="154"/>
     </row>
     <row r="4" spans="1:11" ht="13" customHeight="1">
       <c r="A4" s="150" t="s">
@@ -10398,7 +10492,7 @@
       <c r="B4" s="150" t="s">
         <v>462</v>
       </c>
-      <c r="C4" s="150" t="s">
+      <c r="C4" s="192" t="s">
         <v>475</v>
       </c>
       <c r="D4" s="150">
@@ -10407,10 +10501,10 @@
       <c r="E4" s="150">
         <v>1.98</v>
       </c>
-      <c r="F4" s="180" t="s">
+      <c r="F4" s="159" t="s">
         <v>486</v>
       </c>
-      <c r="G4" s="180" t="s">
+      <c r="G4" s="159" t="s">
         <v>486</v>
       </c>
     </row>
@@ -10421,7 +10515,7 @@
       <c r="B5" s="150" t="s">
         <v>463</v>
       </c>
-      <c r="C5" s="150" t="s">
+      <c r="C5" s="192" t="s">
         <v>474</v>
       </c>
       <c r="D5" s="150">
@@ -10430,33 +10524,33 @@
       <c r="E5" s="150">
         <v>1.1100000000000001</v>
       </c>
-      <c r="F5" s="180" t="s">
+      <c r="F5" s="159" t="s">
         <v>481</v>
       </c>
-      <c r="G5" s="180" t="s">
+      <c r="G5" s="159" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="93" customFormat="1">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="156" t="s">
         <v>490</v>
       </c>
-      <c r="B6" s="176" t="s">
+      <c r="B6" s="156" t="s">
         <v>464</v>
       </c>
-      <c r="C6" s="176" t="s">
+      <c r="C6" s="160" t="s">
         <v>473</v>
       </c>
-      <c r="D6" s="176">
+      <c r="D6" s="156">
         <v>12</v>
       </c>
-      <c r="E6" s="176">
+      <c r="E6" s="156">
         <v>0.49</v>
       </c>
-      <c r="F6" s="181" t="s">
+      <c r="F6" s="160" t="s">
         <v>479</v>
       </c>
-      <c r="G6" s="181" t="s">
+      <c r="G6" s="160" t="s">
         <v>479</v>
       </c>
     </row>
@@ -10467,45 +10561,45 @@
       <c r="B7" s="150" t="s">
         <v>465</v>
       </c>
-      <c r="C7" s="150" t="s">
+      <c r="C7" s="192" t="s">
         <v>472</v>
       </c>
       <c r="D7" s="150">
         <v>16</v>
       </c>
-      <c r="E7" s="180">
+      <c r="E7" s="159">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F7" s="180" t="s">
+      <c r="F7" s="159" t="s">
         <v>480</v>
       </c>
-      <c r="G7" s="180" t="s">
+      <c r="G7" s="159" t="s">
         <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="93" customFormat="1">
-      <c r="A8" s="183"/>
-      <c r="B8" s="183" t="s">
+      <c r="A8" s="162"/>
+      <c r="B8" s="162" t="s">
         <v>482</v>
       </c>
-      <c r="C8" s="183"/>
-      <c r="D8" s="183"/>
-      <c r="E8" s="184">
+      <c r="C8" s="193"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="163">
         <v>0.49</v>
       </c>
-      <c r="F8" s="185" t="s">
+      <c r="F8" s="164" t="s">
         <v>479</v>
       </c>
-      <c r="G8" s="185" t="s">
+      <c r="G8" s="164" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="23" customFormat="1">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
-      <c r="C9" s="177"/>
+      <c r="C9" s="194"/>
       <c r="D9" s="29"/>
-      <c r="E9" s="178"/>
+      <c r="E9" s="157"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
     </row>
@@ -10519,10 +10613,10 @@
       <c r="B11" t="s">
         <v>498</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="155" t="s">
         <v>499</v>
       </c>
-      <c r="D11" s="155" t="s">
+      <c r="D11" s="154" t="s">
         <v>500</v>
       </c>
       <c r="I11" s="94"/>
@@ -10534,7 +10628,7 @@
       <c r="B12" t="s">
         <v>496</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="155" t="s">
         <v>497</v>
       </c>
     </row>
@@ -10566,12 +10660,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C5F8E-5AB4-3747-B9CF-9A1C944F7742}">
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -10602,8 +10696,8 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="F10" s="174"/>
-      <c r="G10" s="174"/>
+      <c r="F10" s="189"/>
+      <c r="G10" s="189"/>
       <c r="I10" t="s">
         <v>453</v>
       </c>
@@ -10644,8 +10738,8 @@
       </c>
     </row>
     <row r="32" spans="2:9">
-      <c r="F32" s="174"/>
-      <c r="G32" s="174"/>
+      <c r="F32" s="189"/>
+      <c r="G32" s="189"/>
       <c r="I32" t="s">
         <v>450</v>
       </c>
@@ -10677,7 +10771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE8B8C4-352E-054D-A843-45DFD254B784}">
   <dimension ref="B2:J61"/>
   <sheetViews>
@@ -10698,10 +10792,10 @@
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="H12" s="175" t="s">
+      <c r="H12" s="190" t="s">
         <v>399</v>
       </c>
-      <c r="I12" s="175"/>
+      <c r="I12" s="190"/>
     </row>
     <row r="14" spans="2:10">
       <c r="J14" t="s">
@@ -10714,10 +10808,10 @@
       </c>
     </row>
     <row r="28" spans="2:9">
-      <c r="H28" s="174" t="s">
+      <c r="H28" s="189" t="s">
         <v>403</v>
       </c>
-      <c r="I28" s="174"/>
+      <c r="I28" s="189"/>
     </row>
     <row r="39" spans="2:9">
       <c r="B39" t="s">
@@ -10725,10 +10819,10 @@
       </c>
     </row>
     <row r="43" spans="2:9">
-      <c r="H43" s="175" t="s">
+      <c r="H43" s="190" t="s">
         <v>406</v>
       </c>
-      <c r="I43" s="175"/>
+      <c r="I43" s="190"/>
     </row>
     <row r="54" spans="2:9">
       <c r="B54" t="s">
@@ -10736,10 +10830,10 @@
       </c>
     </row>
     <row r="59" spans="2:9">
-      <c r="H59" s="174" t="s">
+      <c r="H59" s="189" t="s">
         <v>403</v>
       </c>
-      <c r="I59" s="174"/>
+      <c r="I59" s="189"/>
     </row>
     <row r="61" spans="2:9">
       <c r="G61" t="s">
@@ -10772,15 +10866,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="171" t="s">
         <v>442</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
-      <c r="F1" s="156"/>
-      <c r="G1" s="156"/>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="143" t="s">
@@ -10890,15 +10984,15 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="156" t="s">
+      <c r="A12" s="171" t="s">
         <v>441</v>
       </c>
-      <c r="B12" s="156"/>
-      <c r="C12" s="156"/>
-      <c r="D12" s="156"/>
-      <c r="E12" s="156"/>
-      <c r="F12" s="156"/>
-      <c r="G12" s="156"/>
+      <c r="B12" s="171"/>
+      <c r="C12" s="171"/>
+      <c r="D12" s="171"/>
+      <c r="E12" s="171"/>
+      <c r="F12" s="171"/>
+      <c r="G12" s="171"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="143" t="s">
@@ -13914,7 +14008,7 @@
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="157" t="s">
+      <c r="B5" s="172" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -13934,7 +14028,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="157"/>
+      <c r="B6" s="172"/>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
@@ -13950,7 +14044,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="157"/>
+      <c r="B7" s="172"/>
       <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
@@ -13968,7 +14062,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="157"/>
+      <c r="B8" s="172"/>
       <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
@@ -13986,7 +14080,7 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="157"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="16" t="s">
         <v>33</v>
       </c>
@@ -14004,7 +14098,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="26">
-      <c r="B10" s="157"/>
+      <c r="B10" s="172"/>
       <c r="C10" s="16" t="s">
         <v>13</v>
       </c>
@@ -14022,7 +14116,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="39">
-      <c r="B11" s="158" t="s">
+      <c r="B11" s="173" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -14042,7 +14136,7 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="159"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="15" t="s">
         <v>15</v>
       </c>
@@ -14056,7 +14150,7 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="160"/>
+      <c r="B13" s="175"/>
       <c r="C13" s="15" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Activity can be launched by components from other app
</commit_message>
<xml_diff>
--- a/doc/android.xlsx
+++ b/doc/android.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11014"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B266DA-C7F8-A347-BB87-C3C2FF81D5FB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC657A16-4B15-B945-A3A4-8DDEA3C35504}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="17540" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Android Doc reads" sheetId="16" r:id="rId1"/>
@@ -14,18 +14,19 @@
     <sheet name="Android高级应用开发-深入篇" sheetId="5" r:id="rId4"/>
     <sheet name="反编译" sheetId="8" r:id="rId5"/>
     <sheet name="Android高级应用开发-基础篇_74UI开发的2+1法则" sheetId="1" r:id="rId6"/>
-    <sheet name="版本控制" sheetId="2" r:id="rId7"/>
-    <sheet name="Adapter" sheetId="3" r:id="rId8"/>
-    <sheet name="消息机制" sheetId="6" r:id="rId9"/>
-    <sheet name="消息机制模型" sheetId="10" r:id="rId10"/>
-    <sheet name="基于监听的事件处理机制" sheetId="12" r:id="rId11"/>
-    <sheet name="==与equals" sheetId="7" r:id="rId12"/>
-    <sheet name="hashCode" sheetId="9" r:id="rId13"/>
-    <sheet name="Bitmap.Config" sheetId="20" r:id="rId14"/>
-    <sheet name="drawable_分辨率" sheetId="19" r:id="rId15"/>
-    <sheet name="drawable_2" sheetId="18" r:id="rId16"/>
-    <sheet name="drawable_缩放" sheetId="17" r:id="rId17"/>
-    <sheet name="IO" sheetId="13" r:id="rId18"/>
+    <sheet name="AcrossAppAccess" sheetId="21" r:id="rId7"/>
+    <sheet name="版本控制" sheetId="2" r:id="rId8"/>
+    <sheet name="Adapter" sheetId="3" r:id="rId9"/>
+    <sheet name="消息机制" sheetId="6" r:id="rId10"/>
+    <sheet name="消息机制模型" sheetId="10" r:id="rId11"/>
+    <sheet name="基于监听的事件处理机制" sheetId="12" r:id="rId12"/>
+    <sheet name="==与equals" sheetId="7" r:id="rId13"/>
+    <sheet name="hashCode" sheetId="9" r:id="rId14"/>
+    <sheet name="Bitmap.Config" sheetId="20" r:id="rId15"/>
+    <sheet name="drawable_分辨率" sheetId="19" r:id="rId16"/>
+    <sheet name="drawable_2" sheetId="18" r:id="rId17"/>
+    <sheet name="drawable_缩放" sheetId="17" r:id="rId18"/>
+    <sheet name="IO" sheetId="13" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Android高级应用开发-深入篇'!$A$1:$C$222</definedName>
@@ -99,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="524">
   <si>
     <t>Activity</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2039,12 +2040,47 @@
   <si>
     <t xml:space="preserve"> 1 pixel's Memory (byte)</t>
   </si>
+  <si>
+    <t>Allow other app to start your activity</t>
+  </si>
+  <si>
+    <t>android:exported</t>
+  </si>
+  <si>
+    <t>android:sharedUserId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;intent-filter&gt; </t>
+  </si>
+  <si>
+    <t>java.lang.SecurityException: Permission Denial</t>
+  </si>
+  <si>
+    <t>Activity can be launched by components from other app?</t>
+  </si>
+  <si>
+    <t>HAVE</t>
+  </si>
+  <si>
+    <t>Explicit Intent</t>
+  </si>
+  <si>
+    <t>NOT HAVE</t>
+  </si>
+  <si>
+    <t>1 Explicit Intent
+2 Can not Implicit Intent:ActivityNotFoundException</t>
+  </si>
+  <si>
+    <t>1 Explicit Intent
+2 Implicit Inten</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="39">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2328,6 +2364,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3006,7 +3049,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3327,6 +3370,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3387,18 +3442,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -8872,6 +8919,267 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="B2:U32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:21" ht="16" thickBot="1">
+      <c r="H2" s="69" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21">
+      <c r="G3" s="19"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="21"/>
+    </row>
+    <row r="4" spans="2:21">
+      <c r="G4" s="72" t="s">
+        <v>329</v>
+      </c>
+      <c r="H4" s="73"/>
+      <c r="I4" s="74"/>
+    </row>
+    <row r="5" spans="2:21">
+      <c r="G5" s="72" t="s">
+        <v>328</v>
+      </c>
+      <c r="H5" s="73"/>
+      <c r="I5" s="74"/>
+    </row>
+    <row r="6" spans="2:21" ht="16" thickBot="1">
+      <c r="C6" s="70" t="s">
+        <v>320</v>
+      </c>
+      <c r="E6" s="69" t="s">
+        <v>326</v>
+      </c>
+      <c r="G6" s="72" t="s">
+        <v>331</v>
+      </c>
+      <c r="H6" s="73"/>
+      <c r="I6" s="74"/>
+    </row>
+    <row r="7" spans="2:21" ht="16" thickBot="1">
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
+    </row>
+    <row r="8" spans="2:21">
+      <c r="B8" s="22"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="2:21">
+      <c r="B9" s="22"/>
+      <c r="C9" s="76" t="s">
+        <v>322</v>
+      </c>
+      <c r="D9" s="24"/>
+    </row>
+    <row r="10" spans="2:21">
+      <c r="B10" s="22"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="24"/>
+      <c r="G10" s="79" t="s">
+        <v>335</v>
+      </c>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="79"/>
+      <c r="U10" s="79"/>
+    </row>
+    <row r="11" spans="2:21">
+      <c r="B11" s="22"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="24"/>
+      <c r="G11" s="79" t="s">
+        <v>330</v>
+      </c>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="79"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="79"/>
+      <c r="M11" s="79"/>
+      <c r="N11" s="79"/>
+      <c r="O11" s="79"/>
+      <c r="P11" s="79"/>
+      <c r="Q11" s="79"/>
+      <c r="R11" s="79"/>
+      <c r="S11" s="79"/>
+      <c r="T11" s="79"/>
+      <c r="U11" s="79"/>
+    </row>
+    <row r="12" spans="2:21">
+      <c r="B12" s="22"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="24"/>
+      <c r="G12" s="79" t="s">
+        <v>332</v>
+      </c>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="79"/>
+      <c r="P12" s="79"/>
+      <c r="Q12" s="79"/>
+      <c r="R12" s="79"/>
+      <c r="S12" s="79"/>
+      <c r="T12" s="79"/>
+      <c r="U12" s="79"/>
+    </row>
+    <row r="13" spans="2:21">
+      <c r="B13" s="22"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="24"/>
+    </row>
+    <row r="14" spans="2:21">
+      <c r="B14" s="22"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="24"/>
+    </row>
+    <row r="15" spans="2:21">
+      <c r="B15" s="22"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="24"/>
+      <c r="G15" s="79" t="s">
+        <v>333</v>
+      </c>
+      <c r="H15" s="79"/>
+      <c r="I15" s="79"/>
+      <c r="J15" s="79"/>
+    </row>
+    <row r="16" spans="2:21">
+      <c r="B16" s="22"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="24"/>
+    </row>
+    <row r="17" spans="2:15">
+      <c r="B17" s="22"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="24"/>
+    </row>
+    <row r="18" spans="2:15">
+      <c r="B18" s="22"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="24"/>
+    </row>
+    <row r="19" spans="2:15">
+      <c r="B19" s="22"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="24"/>
+    </row>
+    <row r="20" spans="2:15">
+      <c r="B20" s="22"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="24"/>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="B21" s="22"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="24"/>
+    </row>
+    <row r="22" spans="2:15" ht="16" thickBot="1">
+      <c r="B22" s="22"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="24"/>
+    </row>
+    <row r="23" spans="2:15" ht="16" thickBot="1">
+      <c r="B23" s="22"/>
+      <c r="C23" s="78"/>
+      <c r="D23" s="24"/>
+      <c r="F23" s="66"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="66"/>
+      <c r="I23" s="66"/>
+      <c r="J23" s="66"/>
+    </row>
+    <row r="24" spans="2:15" ht="16" thickBot="1">
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="F24" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="G24" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="H24" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="I24" s="67" t="s">
+        <v>324</v>
+      </c>
+      <c r="J24" s="67" t="s">
+        <v>325</v>
+      </c>
+      <c r="K24" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+    </row>
+    <row r="26" spans="2:15" ht="16" thickBot="1">
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="K28" s="71" t="s">
+        <v>327</v>
+      </c>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="65"/>
+    </row>
+    <row r="32" spans="2:15">
+      <c r="H32" s="79" t="s">
+        <v>334</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA80C652-EB11-2747-89DA-E4ABA79A811D}">
   <dimension ref="A2:T38"/>
   <sheetViews>
@@ -8980,11 +9288,11 @@
       <c r="C6" s="94"/>
       <c r="D6" s="101"/>
       <c r="E6" s="96"/>
-      <c r="F6" s="181" t="s">
+      <c r="F6" s="185" t="s">
         <v>392</v>
       </c>
-      <c r="G6" s="182"/>
-      <c r="H6" s="183"/>
+      <c r="G6" s="186"/>
+      <c r="H6" s="187"/>
       <c r="I6" s="96"/>
       <c r="J6" s="102"/>
       <c r="K6" s="94"/>
@@ -9004,9 +9312,9 @@
       <c r="C7" s="94"/>
       <c r="D7" s="101"/>
       <c r="E7" s="96"/>
-      <c r="F7" s="184"/>
-      <c r="G7" s="185"/>
-      <c r="H7" s="186"/>
+      <c r="F7" s="188"/>
+      <c r="G7" s="189"/>
+      <c r="H7" s="190"/>
       <c r="I7" s="96"/>
       <c r="J7" s="102"/>
       <c r="K7" s="95"/>
@@ -9026,9 +9334,9 @@
       <c r="C8" s="94"/>
       <c r="D8" s="101"/>
       <c r="E8" s="96"/>
-      <c r="F8" s="184"/>
-      <c r="G8" s="185"/>
-      <c r="H8" s="186"/>
+      <c r="F8" s="188"/>
+      <c r="G8" s="189"/>
+      <c r="H8" s="190"/>
       <c r="I8" s="96"/>
       <c r="J8" s="102"/>
       <c r="K8" s="94"/>
@@ -9047,9 +9355,9 @@
       <c r="B9" s="94"/>
       <c r="C9" s="94"/>
       <c r="D9" s="101"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="185"/>
-      <c r="H9" s="186"/>
+      <c r="F9" s="188"/>
+      <c r="G9" s="189"/>
+      <c r="H9" s="190"/>
       <c r="I9" s="96"/>
       <c r="J9" s="102"/>
       <c r="K9" s="94"/>
@@ -9068,9 +9376,9 @@
       <c r="B10" s="94"/>
       <c r="C10" s="94"/>
       <c r="D10" s="101"/>
-      <c r="F10" s="187"/>
-      <c r="G10" s="188"/>
-      <c r="H10" s="189"/>
+      <c r="F10" s="191"/>
+      <c r="G10" s="192"/>
+      <c r="H10" s="193"/>
       <c r="I10" s="129"/>
       <c r="J10" s="102"/>
       <c r="K10" s="94"/>
@@ -9662,7 +9970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7778B8-D430-A34A-995E-0F83AC473C52}">
   <dimension ref="E8:K35"/>
   <sheetViews>
@@ -9742,16 +10050,16 @@
     </row>
     <row r="18" spans="5:8">
       <c r="E18" s="137"/>
-      <c r="F18" s="190" t="s">
+      <c r="F18" s="194" t="s">
         <v>395</v>
       </c>
-      <c r="G18" s="191"/>
+      <c r="G18" s="195"/>
       <c r="H18" s="135"/>
     </row>
     <row r="19" spans="5:8">
       <c r="E19" s="137"/>
-      <c r="F19" s="192"/>
-      <c r="G19" s="193"/>
+      <c r="F19" s="196"/>
+      <c r="G19" s="197"/>
       <c r="H19" s="135"/>
     </row>
     <row r="20" spans="5:8">
@@ -9847,7 +10155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:K25"/>
   <sheetViews>
@@ -10062,7 +10370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A3:E21"/>
   <sheetViews>
@@ -10245,11 +10553,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFDE749-2C0C-C548-8C4F-6EF43EA89AA0}">
   <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -10260,7 +10568,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="176" t="s">
         <v>506</v>
       </c>
       <c r="C2" s="151" t="s">
@@ -10268,7 +10576,7 @@
       </c>
     </row>
     <row r="3" spans="2:3">
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="177" t="s">
         <v>505</v>
       </c>
       <c r="C3" s="150">
@@ -10276,7 +10584,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="32">
-      <c r="B4" s="199" t="s">
+      <c r="B4" s="179" t="s">
         <v>511</v>
       </c>
       <c r="C4" s="150">
@@ -10284,7 +10592,7 @@
       </c>
     </row>
     <row r="5" spans="2:3">
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="177" t="s">
         <v>507</v>
       </c>
       <c r="C5" s="150">
@@ -10292,15 +10600,15 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="197" t="s">
+      <c r="B6" s="177" t="s">
         <v>508</v>
       </c>
-      <c r="C6" s="198" t="s">
+      <c r="C6" s="178" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="7" spans="2:3">
-      <c r="B7" s="197" t="s">
+      <c r="B7" s="177" t="s">
         <v>509</v>
       </c>
       <c r="C7" s="150">
@@ -10308,7 +10616,7 @@
       </c>
     </row>
     <row r="8" spans="2:3">
-      <c r="B8" s="197" t="s">
+      <c r="B8" s="177" t="s">
         <v>510</v>
       </c>
       <c r="C8" s="150">
@@ -10323,7 +10631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86ED6A2-BD47-244B-AD18-088367512271}">
   <dimension ref="B2:M10"/>
   <sheetViews>
@@ -10427,7 +10735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A51D4780-106D-3C46-B51D-1FAF5E0D4E2A}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -10694,7 +11002,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C5F8E-5AB4-3747-B9CF-9A1C944F7742}">
   <dimension ref="A1:I35"/>
   <sheetViews>
@@ -10730,8 +11038,8 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="F10" s="194"/>
-      <c r="G10" s="194"/>
+      <c r="F10" s="198"/>
+      <c r="G10" s="198"/>
       <c r="I10" t="s">
         <v>453</v>
       </c>
@@ -10772,8 +11080,8 @@
       </c>
     </row>
     <row r="32" spans="2:9">
-      <c r="F32" s="194"/>
-      <c r="G32" s="194"/>
+      <c r="F32" s="198"/>
+      <c r="G32" s="198"/>
       <c r="I32" t="s">
         <v>450</v>
       </c>
@@ -10805,7 +11113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE8B8C4-352E-054D-A843-45DFD254B784}">
   <dimension ref="B2:J61"/>
   <sheetViews>
@@ -10826,10 +11134,10 @@
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="H12" s="195" t="s">
+      <c r="H12" s="199" t="s">
         <v>399</v>
       </c>
-      <c r="I12" s="195"/>
+      <c r="I12" s="199"/>
     </row>
     <row r="14" spans="2:10">
       <c r="J14" t="s">
@@ -10842,10 +11150,10 @@
       </c>
     </row>
     <row r="28" spans="2:9">
-      <c r="H28" s="194" t="s">
+      <c r="H28" s="198" t="s">
         <v>403</v>
       </c>
-      <c r="I28" s="194"/>
+      <c r="I28" s="198"/>
     </row>
     <row r="39" spans="2:9">
       <c r="B39" t="s">
@@ -10853,10 +11161,10 @@
       </c>
     </row>
     <row r="43" spans="2:9">
-      <c r="H43" s="195" t="s">
+      <c r="H43" s="199" t="s">
         <v>406</v>
       </c>
-      <c r="I43" s="195"/>
+      <c r="I43" s="199"/>
     </row>
     <row r="54" spans="2:9">
       <c r="B54" t="s">
@@ -10864,10 +11172,10 @@
       </c>
     </row>
     <row r="59" spans="2:9">
-      <c r="H59" s="194" t="s">
+      <c r="H59" s="198" t="s">
         <v>403</v>
       </c>
-      <c r="I59" s="194"/>
+      <c r="I59" s="198"/>
     </row>
     <row r="61" spans="2:9">
       <c r="G61" t="s">
@@ -10900,15 +11208,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="180" t="s">
         <v>442</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="G1" s="180"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="143" t="s">
@@ -11018,15 +11326,15 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="180" t="s">
         <v>441</v>
       </c>
-      <c r="B12" s="176"/>
-      <c r="C12" s="176"/>
-      <c r="D12" s="176"/>
-      <c r="E12" s="176"/>
-      <c r="F12" s="176"/>
-      <c r="G12" s="176"/>
+      <c r="B12" s="180"/>
+      <c r="C12" s="180"/>
+      <c r="D12" s="180"/>
+      <c r="E12" s="180"/>
+      <c r="F12" s="180"/>
+      <c r="G12" s="180"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="143" t="s">
@@ -13987,6 +14295,122 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0C945C-04F2-D147-89E5-6DDFCFB3EEA7}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="52.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="199" t="s">
+        <v>513</v>
+      </c>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
+      <c r="D1" s="199"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="143" t="s">
+        <v>514</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>515</v>
+      </c>
+      <c r="C2" s="143" t="s">
+        <v>516</v>
+      </c>
+      <c r="D2" s="143" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="144" t="b">
+        <v>0</v>
+      </c>
+      <c r="B3" s="144" t="s">
+        <v>521</v>
+      </c>
+      <c r="C3" s="144" t="s">
+        <v>521</v>
+      </c>
+      <c r="D3" s="201" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="144" t="b">
+        <v>0</v>
+      </c>
+      <c r="B4" s="144" t="s">
+        <v>519</v>
+      </c>
+      <c r="C4" s="144" t="s">
+        <v>521</v>
+      </c>
+      <c r="D4" s="144" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="144" t="b">
+        <v>0</v>
+      </c>
+      <c r="B5" s="144" t="s">
+        <v>521</v>
+      </c>
+      <c r="C5" s="144" t="s">
+        <v>519</v>
+      </c>
+      <c r="D5" s="201" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="32">
+      <c r="A6" s="144" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="144" t="s">
+        <v>521</v>
+      </c>
+      <c r="C6" s="144" t="s">
+        <v>521</v>
+      </c>
+      <c r="D6" s="200" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="32">
+      <c r="A7" s="144" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="144" t="s">
+        <v>521</v>
+      </c>
+      <c r="C7" s="144" t="s">
+        <v>519</v>
+      </c>
+      <c r="D7" s="200" t="s">
+        <v>523</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:G13"/>
   <sheetViews>
@@ -14042,7 +14466,7 @@
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="177" t="s">
+      <c r="B5" s="181" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -14062,7 +14486,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="177"/>
+      <c r="B6" s="181"/>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
@@ -14078,7 +14502,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="177"/>
+      <c r="B7" s="181"/>
       <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
@@ -14096,7 +14520,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="177"/>
+      <c r="B8" s="181"/>
       <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
@@ -14114,7 +14538,7 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="177"/>
+      <c r="B9" s="181"/>
       <c r="C9" s="16" t="s">
         <v>33</v>
       </c>
@@ -14132,7 +14556,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="26">
-      <c r="B10" s="177"/>
+      <c r="B10" s="181"/>
       <c r="C10" s="16" t="s">
         <v>13</v>
       </c>
@@ -14150,7 +14574,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="39">
-      <c r="B11" s="178" t="s">
+      <c r="B11" s="182" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -14170,7 +14594,7 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="179"/>
+      <c r="B12" s="183"/>
       <c r="C12" s="15" t="s">
         <v>15</v>
       </c>
@@ -14184,7 +14608,7 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="180"/>
+      <c r="B13" s="184"/>
       <c r="C13" s="15" t="s">
         <v>16</v>
       </c>
@@ -14210,7 +14634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:N24"/>
   <sheetViews>
@@ -14368,265 +14792,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B2:U32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:21" ht="16" thickBot="1">
-      <c r="H2" s="69" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="3" spans="2:21">
-      <c r="G3" s="19"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
-    </row>
-    <row r="4" spans="2:21">
-      <c r="G4" s="72" t="s">
-        <v>329</v>
-      </c>
-      <c r="H4" s="73"/>
-      <c r="I4" s="74"/>
-    </row>
-    <row r="5" spans="2:21">
-      <c r="G5" s="72" t="s">
-        <v>328</v>
-      </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="74"/>
-    </row>
-    <row r="6" spans="2:21" ht="16" thickBot="1">
-      <c r="C6" s="70" t="s">
-        <v>320</v>
-      </c>
-      <c r="E6" s="69" t="s">
-        <v>326</v>
-      </c>
-      <c r="G6" s="72" t="s">
-        <v>331</v>
-      </c>
-      <c r="H6" s="73"/>
-      <c r="I6" s="74"/>
-    </row>
-    <row r="7" spans="2:21" ht="16" thickBot="1">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-    </row>
-    <row r="8" spans="2:21">
-      <c r="B8" s="22"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="24"/>
-    </row>
-    <row r="9" spans="2:21">
-      <c r="B9" s="22"/>
-      <c r="C9" s="76" t="s">
-        <v>322</v>
-      </c>
-      <c r="D9" s="24"/>
-    </row>
-    <row r="10" spans="2:21">
-      <c r="B10" s="22"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="24"/>
-      <c r="G10" s="79" t="s">
-        <v>335</v>
-      </c>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79"/>
-      <c r="M10" s="79"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="79"/>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="79"/>
-      <c r="R10" s="79"/>
-      <c r="S10" s="79"/>
-      <c r="T10" s="79"/>
-      <c r="U10" s="79"/>
-    </row>
-    <row r="11" spans="2:21">
-      <c r="B11" s="22"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="24"/>
-      <c r="G11" s="79" t="s">
-        <v>330</v>
-      </c>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="79"/>
-      <c r="N11" s="79"/>
-      <c r="O11" s="79"/>
-      <c r="P11" s="79"/>
-      <c r="Q11" s="79"/>
-      <c r="R11" s="79"/>
-      <c r="S11" s="79"/>
-      <c r="T11" s="79"/>
-      <c r="U11" s="79"/>
-    </row>
-    <row r="12" spans="2:21">
-      <c r="B12" s="22"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="24"/>
-      <c r="G12" s="79" t="s">
-        <v>332</v>
-      </c>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
-      <c r="N12" s="79"/>
-      <c r="O12" s="79"/>
-      <c r="P12" s="79"/>
-      <c r="Q12" s="79"/>
-      <c r="R12" s="79"/>
-      <c r="S12" s="79"/>
-      <c r="T12" s="79"/>
-      <c r="U12" s="79"/>
-    </row>
-    <row r="13" spans="2:21">
-      <c r="B13" s="22"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="24"/>
-    </row>
-    <row r="14" spans="2:21">
-      <c r="B14" s="22"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="24"/>
-    </row>
-    <row r="15" spans="2:21">
-      <c r="B15" s="22"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="24"/>
-      <c r="G15" s="79" t="s">
-        <v>333</v>
-      </c>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="79"/>
-    </row>
-    <row r="16" spans="2:21">
-      <c r="B16" s="22"/>
-      <c r="C16" s="77"/>
-      <c r="D16" s="24"/>
-    </row>
-    <row r="17" spans="2:15">
-      <c r="B17" s="22"/>
-      <c r="C17" s="77"/>
-      <c r="D17" s="24"/>
-    </row>
-    <row r="18" spans="2:15">
-      <c r="B18" s="22"/>
-      <c r="C18" s="77"/>
-      <c r="D18" s="24"/>
-    </row>
-    <row r="19" spans="2:15">
-      <c r="B19" s="22"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="24"/>
-    </row>
-    <row r="20" spans="2:15">
-      <c r="B20" s="22"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="24"/>
-    </row>
-    <row r="21" spans="2:15">
-      <c r="B21" s="22"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="24"/>
-    </row>
-    <row r="22" spans="2:15" ht="16" thickBot="1">
-      <c r="B22" s="22"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="24"/>
-    </row>
-    <row r="23" spans="2:15" ht="16" thickBot="1">
-      <c r="B23" s="22"/>
-      <c r="C23" s="78"/>
-      <c r="D23" s="24"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="66"/>
-    </row>
-    <row r="24" spans="2:15" ht="16" thickBot="1">
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="27"/>
-      <c r="F24" s="67" t="s">
-        <v>324</v>
-      </c>
-      <c r="G24" s="67" t="s">
-        <v>324</v>
-      </c>
-      <c r="H24" s="67" t="s">
-        <v>324</v>
-      </c>
-      <c r="I24" s="67" t="s">
-        <v>324</v>
-      </c>
-      <c r="J24" s="67" t="s">
-        <v>325</v>
-      </c>
-      <c r="K24" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15">
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-    </row>
-    <row r="26" spans="2:15" ht="16" thickBot="1">
-      <c r="F26" s="68"/>
-      <c r="G26" s="68"/>
-      <c r="H26" s="68"/>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-    </row>
-    <row r="28" spans="2:15">
-      <c r="K28" s="71" t="s">
-        <v>327</v>
-      </c>
-      <c r="L28" s="71"/>
-      <c r="M28" s="71"/>
-      <c r="N28" s="71"/>
-      <c r="O28" s="65"/>
-    </row>
-    <row r="32" spans="2:15">
-      <c r="H32" s="79" t="s">
-        <v>334</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Access Remote Activity using ImplicitIntent
</commit_message>
<xml_diff>
--- a/doc/android.xlsx
+++ b/doc/android.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F405593-4CE4-D84F-B802-000CD66AA7E7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112D03DC-6806-EE44-9360-690DE73642EF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="531">
   <si>
     <t>Activity</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2024,9 +2024,6 @@
     <t>android:exported</t>
   </si>
   <si>
-    <t>android:sharedUserId</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;intent-filter&gt; </t>
   </si>
   <si>
@@ -2049,47 +2046,68 @@
 2 Can not Implicit Intent:ActivityNotFoundException</t>
   </si>
   <si>
+    <t>Sheet name</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Allow Other App To Start your Activity</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>LruCache&lt;String, BitmapDrawable&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disk Cacche</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Network</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memory Cache</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Client</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>android:sharedUserId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Same Signature + sharedUserId</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Signature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>1 Explicit Intent
 2 Implicit Inten</t>
-  </si>
-  <si>
-    <t>Sheet name</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Allow Other App To Start your Activity</t>
-  </si>
-  <si>
-    <t>Home</t>
-  </si>
-  <si>
-    <t>LruCache&lt;String, BitmapDrawable&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>UI</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Disk Cacche</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Network</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Memory Cache</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Client</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>✅</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Implicit Intent</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2097,7 +2115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="44">
+  <fonts count="45">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2423,6 +2441,12 @@
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3185,7 +3209,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3555,6 +3579,7 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3618,7 +3643,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -9997,15 +10022,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B2" s="183"/>
     </row>
@@ -10545,11 +10570,11 @@
       <c r="C6" s="94"/>
       <c r="D6" s="101"/>
       <c r="E6" s="96"/>
-      <c r="F6" s="207" t="s">
+      <c r="F6" s="208" t="s">
         <v>392</v>
       </c>
-      <c r="G6" s="208"/>
-      <c r="H6" s="209"/>
+      <c r="G6" s="209"/>
+      <c r="H6" s="210"/>
       <c r="I6" s="96"/>
       <c r="J6" s="102"/>
       <c r="K6" s="94"/>
@@ -10569,9 +10594,9 @@
       <c r="C7" s="94"/>
       <c r="D7" s="101"/>
       <c r="E7" s="96"/>
-      <c r="F7" s="210"/>
-      <c r="G7" s="211"/>
-      <c r="H7" s="212"/>
+      <c r="F7" s="211"/>
+      <c r="G7" s="212"/>
+      <c r="H7" s="213"/>
       <c r="I7" s="96"/>
       <c r="J7" s="102"/>
       <c r="K7" s="95"/>
@@ -10591,9 +10616,9 @@
       <c r="C8" s="94"/>
       <c r="D8" s="101"/>
       <c r="E8" s="96"/>
-      <c r="F8" s="210"/>
-      <c r="G8" s="211"/>
-      <c r="H8" s="212"/>
+      <c r="F8" s="211"/>
+      <c r="G8" s="212"/>
+      <c r="H8" s="213"/>
       <c r="I8" s="96"/>
       <c r="J8" s="102"/>
       <c r="K8" s="94"/>
@@ -10612,9 +10637,9 @@
       <c r="B9" s="94"/>
       <c r="C9" s="94"/>
       <c r="D9" s="101"/>
-      <c r="F9" s="210"/>
-      <c r="G9" s="211"/>
-      <c r="H9" s="212"/>
+      <c r="F9" s="211"/>
+      <c r="G9" s="212"/>
+      <c r="H9" s="213"/>
       <c r="I9" s="96"/>
       <c r="J9" s="102"/>
       <c r="K9" s="94"/>
@@ -10633,9 +10658,9 @@
       <c r="B10" s="94"/>
       <c r="C10" s="94"/>
       <c r="D10" s="101"/>
-      <c r="F10" s="213"/>
-      <c r="G10" s="214"/>
-      <c r="H10" s="215"/>
+      <c r="F10" s="214"/>
+      <c r="G10" s="215"/>
+      <c r="H10" s="216"/>
       <c r="I10" s="129"/>
       <c r="J10" s="102"/>
       <c r="K10" s="94"/>
@@ -11308,16 +11333,16 @@
     </row>
     <row r="18" spans="5:8">
       <c r="E18" s="137"/>
-      <c r="F18" s="216" t="s">
+      <c r="F18" s="217" t="s">
         <v>395</v>
       </c>
-      <c r="G18" s="217"/>
+      <c r="G18" s="218"/>
       <c r="H18" s="135"/>
     </row>
     <row r="19" spans="5:8">
       <c r="E19" s="137"/>
-      <c r="F19" s="218"/>
-      <c r="G19" s="219"/>
+      <c r="F19" s="219"/>
+      <c r="G19" s="220"/>
       <c r="H19" s="135"/>
     </row>
     <row r="20" spans="5:8">
@@ -12300,8 +12325,8 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="F10" s="220"/>
-      <c r="G10" s="220"/>
+      <c r="F10" s="221"/>
+      <c r="G10" s="221"/>
       <c r="I10" t="s">
         <v>445</v>
       </c>
@@ -12342,8 +12367,8 @@
       </c>
     </row>
     <row r="32" spans="2:9">
-      <c r="F32" s="220"/>
-      <c r="G32" s="220"/>
+      <c r="F32" s="221"/>
+      <c r="G32" s="221"/>
       <c r="I32" t="s">
         <v>442</v>
       </c>
@@ -12395,19 +12420,19 @@
   <sheetData>
     <row r="1" spans="1:19" s="199" customFormat="1" ht="18" thickBot="1">
       <c r="A1" s="199" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F1" s="199" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="N1" s="200"/>
       <c r="O1" s="200" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="P1" s="200"/>
       <c r="Q1" s="200"/>
       <c r="S1" s="199" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -12423,7 +12448,7 @@
       <c r="D3" s="194"/>
       <c r="E3" s="23"/>
       <c r="F3" s="188" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -12670,7 +12695,7 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
   </sheetData>
@@ -12701,10 +12726,10 @@
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="H12" s="221" t="s">
+      <c r="H12" s="222" t="s">
         <v>399</v>
       </c>
-      <c r="I12" s="221"/>
+      <c r="I12" s="222"/>
     </row>
     <row r="14" spans="2:10">
       <c r="J14" t="s">
@@ -12717,10 +12742,10 @@
       </c>
     </row>
     <row r="28" spans="2:9">
-      <c r="H28" s="220" t="s">
+      <c r="H28" s="221" t="s">
         <v>403</v>
       </c>
-      <c r="I28" s="220"/>
+      <c r="I28" s="221"/>
     </row>
     <row r="39" spans="2:9">
       <c r="B39" t="s">
@@ -12728,10 +12753,10 @@
       </c>
     </row>
     <row r="43" spans="2:9">
-      <c r="H43" s="221" t="s">
+      <c r="H43" s="222" t="s">
         <v>406</v>
       </c>
-      <c r="I43" s="221"/>
+      <c r="I43" s="222"/>
     </row>
     <row r="54" spans="2:9">
       <c r="B54" t="s">
@@ -12739,10 +12764,10 @@
       </c>
     </row>
     <row r="59" spans="2:9">
-      <c r="H59" s="220" t="s">
+      <c r="H59" s="221" t="s">
         <v>403</v>
       </c>
-      <c r="I59" s="220"/>
+      <c r="I59" s="221"/>
     </row>
     <row r="61" spans="2:9">
       <c r="G61" t="s">
@@ -12764,126 +12789,163 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0C945C-04F2-D147-89E5-6DDFCFB3EEA7}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="52.5" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="52.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="147" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="18">
-      <c r="A2" s="201" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18">
+      <c r="A2" s="202" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="201"/>
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2" s="202"/>
+      <c r="C2" s="202"/>
+      <c r="D2" s="202"/>
+      <c r="E2" s="202"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="143" t="s">
         <v>506</v>
       </c>
       <c r="B3" s="143" t="s">
+        <v>525</v>
+      </c>
+      <c r="C3" s="143" t="s">
+        <v>527</v>
+      </c>
+      <c r="D3" s="143" t="s">
         <v>507</v>
       </c>
-      <c r="C3" s="143" t="s">
-        <v>508</v>
-      </c>
-      <c r="D3" s="143" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="143" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="144" t="b">
         <v>0</v>
       </c>
       <c r="B4" s="144" t="s">
-        <v>513</v>
-      </c>
-      <c r="C4" s="144" t="s">
-        <v>513</v>
-      </c>
-      <c r="D4" s="181" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>512</v>
+      </c>
+      <c r="C4" s="144"/>
+      <c r="D4" s="144" t="s">
+        <v>512</v>
+      </c>
+      <c r="E4" s="181" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="144" t="b">
         <v>0</v>
       </c>
       <c r="B5" s="144" t="s">
-        <v>511</v>
-      </c>
-      <c r="C5" s="144" t="s">
-        <v>513</v>
-      </c>
+        <v>510</v>
+      </c>
+      <c r="C5" s="144"/>
       <c r="D5" s="144" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="144" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="144" t="b">
         <v>0</v>
       </c>
       <c r="B6" s="144" t="s">
-        <v>513</v>
-      </c>
-      <c r="C6" s="144" t="s">
-        <v>511</v>
-      </c>
-      <c r="D6" s="181" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="30">
+        <v>512</v>
+      </c>
+      <c r="C6" s="144"/>
+      <c r="D6" s="144" t="s">
+        <v>510</v>
+      </c>
+      <c r="E6" s="181" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="144" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="144" t="s">
-        <v>513</v>
-      </c>
-      <c r="C7" s="144" t="s">
-        <v>513</v>
-      </c>
-      <c r="D7" s="180" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="30">
+        <v>512</v>
+      </c>
+      <c r="C7" s="145" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="144" t="s">
+        <v>510</v>
+      </c>
+      <c r="E7" s="223" t="s">
+        <v>530</v>
+      </c>
+      <c r="F7" s="201" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30">
       <c r="A8" s="144" t="b">
         <v>1</v>
       </c>
       <c r="B8" s="144" t="s">
+        <v>512</v>
+      </c>
+      <c r="C8" s="144"/>
+      <c r="D8" s="144" t="s">
+        <v>512</v>
+      </c>
+      <c r="E8" s="180" t="s">
         <v>513</v>
       </c>
-      <c r="C8" s="144" t="s">
-        <v>511</v>
-      </c>
-      <c r="D8" s="180" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9" s="222" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="144" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="144" t="s">
+        <v>512</v>
+      </c>
+      <c r="C9" s="144"/>
+      <c r="D9" s="144" t="s">
+        <v>510</v>
+      </c>
+      <c r="E9" s="180" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="201" t="s">
+        <v>524</v>
+      </c>
+      <c r="C10" s="201"/>
+      <c r="D10" s="201"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="B11" s="201" t="s">
         <v>526</v>
       </c>
-      <c r="C9" s="222"/>
+      <c r="C11" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A2:E2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -12907,15 +12969,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="202" t="s">
+      <c r="A1" s="203" t="s">
         <v>434</v>
       </c>
-      <c r="B1" s="202"/>
-      <c r="C1" s="202"/>
-      <c r="D1" s="202"/>
-      <c r="E1" s="202"/>
-      <c r="F1" s="202"/>
-      <c r="G1" s="202"/>
+      <c r="B1" s="203"/>
+      <c r="C1" s="203"/>
+      <c r="D1" s="203"/>
+      <c r="E1" s="203"/>
+      <c r="F1" s="203"/>
+      <c r="G1" s="203"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="143" t="s">
@@ -13025,15 +13087,15 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="202" t="s">
+      <c r="A12" s="203" t="s">
         <v>433</v>
       </c>
-      <c r="B12" s="202"/>
-      <c r="C12" s="202"/>
-      <c r="D12" s="202"/>
-      <c r="E12" s="202"/>
-      <c r="F12" s="202"/>
-      <c r="G12" s="202"/>
+      <c r="B12" s="203"/>
+      <c r="C12" s="203"/>
+      <c r="D12" s="203"/>
+      <c r="E12" s="203"/>
+      <c r="F12" s="203"/>
+      <c r="G12" s="203"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="143" t="s">
@@ -16050,7 +16112,7 @@
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="203" t="s">
+      <c r="B5" s="204" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -16070,7 +16132,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="203"/>
+      <c r="B6" s="204"/>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
@@ -16086,7 +16148,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="203"/>
+      <c r="B7" s="204"/>
       <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
@@ -16104,7 +16166,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="203"/>
+      <c r="B8" s="204"/>
       <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
@@ -16122,7 +16184,7 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="203"/>
+      <c r="B9" s="204"/>
       <c r="C9" s="16" t="s">
         <v>33</v>
       </c>
@@ -16140,7 +16202,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="28">
-      <c r="B10" s="203"/>
+      <c r="B10" s="204"/>
       <c r="C10" s="16" t="s">
         <v>13</v>
       </c>
@@ -16158,7 +16220,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="42">
-      <c r="B11" s="204" t="s">
+      <c r="B11" s="205" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -16178,7 +16240,7 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="205"/>
+      <c r="B12" s="206"/>
       <c r="C12" s="15" t="s">
         <v>15</v>
       </c>
@@ -16192,7 +16254,7 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="206"/>
+      <c r="B13" s="207"/>
       <c r="C13" s="15" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
add Room test case
</commit_message>
<xml_diff>
--- a/doc/android.xlsx
+++ b/doc/android.xlsx
@@ -3,36 +3,37 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CD28D5-C7E9-9C49-880B-9DEC494B840E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704281B2-E63B-8040-860F-1DC73979E0C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="16" r:id="rId1"/>
-    <sheet name="DB" sheetId="23" r:id="rId2"/>
-    <sheet name="ThreeeLevelCache" sheetId="22" r:id="rId3"/>
-    <sheet name="IPC" sheetId="21" r:id="rId4"/>
-    <sheet name="Activity_Lifecycle" sheetId="15" r:id="rId5"/>
-    <sheet name="ContentProvider" sheetId="4" r:id="rId6"/>
-    <sheet name="Android高级应用开发-深入篇" sheetId="5" r:id="rId7"/>
-    <sheet name="反编译" sheetId="8" r:id="rId8"/>
-    <sheet name="Android高级应用开发-基础篇_74UI开发的2+1法则" sheetId="1" r:id="rId9"/>
-    <sheet name="版本控制" sheetId="2" r:id="rId10"/>
-    <sheet name="Adapter" sheetId="3" r:id="rId11"/>
-    <sheet name="消息机制" sheetId="6" r:id="rId12"/>
-    <sheet name="消息机制模型" sheetId="10" r:id="rId13"/>
-    <sheet name="基于监听的事件处理机制" sheetId="12" r:id="rId14"/>
-    <sheet name="==与equals" sheetId="7" r:id="rId15"/>
-    <sheet name="hashCode" sheetId="9" r:id="rId16"/>
-    <sheet name="Bitmap.Config" sheetId="20" r:id="rId17"/>
-    <sheet name="drawable_分辨率" sheetId="19" r:id="rId18"/>
-    <sheet name="drawable_2" sheetId="18" r:id="rId19"/>
-    <sheet name="drawable_缩放" sheetId="17" r:id="rId20"/>
-    <sheet name="IO" sheetId="13" r:id="rId21"/>
+    <sheet name="DB_Room" sheetId="24" r:id="rId2"/>
+    <sheet name="DB" sheetId="23" r:id="rId3"/>
+    <sheet name="ThreeeLevelCache" sheetId="22" r:id="rId4"/>
+    <sheet name="IPC" sheetId="21" r:id="rId5"/>
+    <sheet name="Activity_Lifecycle" sheetId="15" r:id="rId6"/>
+    <sheet name="ContentProvider" sheetId="4" r:id="rId7"/>
+    <sheet name="Android高级应用开发-深入篇" sheetId="5" r:id="rId8"/>
+    <sheet name="反编译" sheetId="8" r:id="rId9"/>
+    <sheet name="Android高级应用开发-基础篇_74UI开发的2+1法则" sheetId="1" r:id="rId10"/>
+    <sheet name="版本控制" sheetId="2" r:id="rId11"/>
+    <sheet name="Adapter" sheetId="3" r:id="rId12"/>
+    <sheet name="消息机制" sheetId="6" r:id="rId13"/>
+    <sheet name="消息机制模型" sheetId="10" r:id="rId14"/>
+    <sheet name="基于监听的事件处理机制" sheetId="12" r:id="rId15"/>
+    <sheet name="==与equals" sheetId="7" r:id="rId16"/>
+    <sheet name="hashCode" sheetId="9" r:id="rId17"/>
+    <sheet name="Bitmap.Config" sheetId="20" r:id="rId18"/>
+    <sheet name="drawable_分辨率" sheetId="19" r:id="rId19"/>
+    <sheet name="drawable_2" sheetId="18" r:id="rId20"/>
+    <sheet name="drawable_缩放" sheetId="17" r:id="rId21"/>
+    <sheet name="IO" sheetId="13" r:id="rId22"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Android高级应用开发-深入篇'!$A$1:$C$222</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'Android高级应用开发-深入篇'!$A$1:$D$225</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Android高级应用开发-深入篇'!$A$1:$C$222</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">'Android高级应用开发-深入篇'!$A$1:$D$225</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
 </workbook>
@@ -102,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="579">
   <si>
     <t>Activity</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2243,12 +2244,72 @@
     <t>测试设备：SamSung S8 Android 8.0</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>DB_Room</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Course(course)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>course_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>course_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Primary key</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foriengin key</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Student(stu)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stu_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stu_name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Score</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>score</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agile</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="46">
+  <fonts count="47">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2589,8 +2650,15 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.39997558519241921"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2642,6 +2710,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3361,7 +3441,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="232">
+  <cellXfs count="239">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3750,6 +3830,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3813,7 +3894,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="46" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -10239,10 +10330,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD58857B-D0A1-5746-959D-8AF492D5EE51}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -10272,16 +10363,356 @@
         <v>531</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B4" s="147" t="s">
+        <v>564</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3" location="DB!A1" display="DB" xr:uid="{E442FB97-6815-464C-B9AA-C4CE8E614689}"/>
+    <hyperlink ref="B4" location="DB_Room!A1" display="DB_Room" xr:uid="{BB703428-235E-F14D-B13E-18D1983CAF4E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:Q39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16" width="9" style="1"/>
+    <col min="17" max="17" width="68.6640625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:17">
+      <c r="C1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="2:17" ht="14" thickBot="1">
+      <c r="D2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="C4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="H4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="M4" s="6"/>
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="C5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="H5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="M5" s="6"/>
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="C6" s="6"/>
+      <c r="E6" s="7"/>
+      <c r="H6" s="6"/>
+      <c r="J6" s="7"/>
+      <c r="M6" s="6"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="C7" s="6"/>
+      <c r="E7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="J7" s="7"/>
+      <c r="M7" s="6"/>
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="2:17" ht="14" thickBot="1">
+      <c r="C8" s="6"/>
+      <c r="E8" s="7"/>
+      <c r="H8" s="6"/>
+      <c r="J8" s="7"/>
+      <c r="M8" s="6"/>
+      <c r="O8" s="7"/>
+    </row>
+    <row r="9" spans="2:17" ht="29" thickBot="1">
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="7"/>
+      <c r="Q9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="C10" s="6"/>
+      <c r="E10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="J10" s="7"/>
+      <c r="M10" s="6"/>
+      <c r="O10" s="7"/>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="C11" s="6"/>
+      <c r="E11" s="7"/>
+      <c r="H11" s="6"/>
+      <c r="J11" s="7"/>
+      <c r="M11" s="6"/>
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="C12" s="6"/>
+      <c r="E12" s="7"/>
+      <c r="H12" s="6"/>
+      <c r="J12" s="7"/>
+      <c r="M12" s="6"/>
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="C13" s="6"/>
+      <c r="E13" s="7"/>
+      <c r="H13" s="6"/>
+      <c r="J13" s="7"/>
+      <c r="M13" s="6"/>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="C14" s="6"/>
+      <c r="E14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="J14" s="7"/>
+      <c r="M14" s="6"/>
+      <c r="O14" s="7"/>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="C15" s="6"/>
+      <c r="E15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="J15" s="7"/>
+      <c r="M15" s="6"/>
+      <c r="O15" s="7"/>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="C16" s="6"/>
+      <c r="E16" s="7"/>
+      <c r="H16" s="6"/>
+      <c r="J16" s="7"/>
+      <c r="M16" s="6"/>
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="2:17" ht="14" thickBot="1">
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="11"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="11"/>
+    </row>
+    <row r="24" spans="2:17" ht="14" thickBot="1">
+      <c r="D24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17">
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="2:17">
+      <c r="C26" s="6"/>
+      <c r="E26" s="7"/>
+      <c r="H26" s="6"/>
+      <c r="J26" s="7"/>
+      <c r="M26" s="6"/>
+      <c r="O26" s="7"/>
+    </row>
+    <row r="27" spans="2:17">
+      <c r="C27" s="6"/>
+      <c r="E27" s="7"/>
+      <c r="H27" s="6"/>
+      <c r="J27" s="7"/>
+      <c r="M27" s="6"/>
+      <c r="O27" s="7"/>
+    </row>
+    <row r="28" spans="2:17">
+      <c r="C28" s="6"/>
+      <c r="E28" s="7"/>
+      <c r="H28" s="6"/>
+      <c r="J28" s="7"/>
+      <c r="M28" s="6"/>
+      <c r="O28" s="7"/>
+    </row>
+    <row r="29" spans="2:17">
+      <c r="C29" s="6"/>
+      <c r="E29" s="7"/>
+      <c r="H29" s="6"/>
+      <c r="J29" s="7"/>
+      <c r="M29" s="6"/>
+      <c r="O29" s="7"/>
+    </row>
+    <row r="30" spans="2:17">
+      <c r="C30" s="6"/>
+      <c r="E30" s="7"/>
+      <c r="H30" s="6"/>
+      <c r="J30" s="7"/>
+      <c r="M30" s="6"/>
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="2:17" ht="42">
+      <c r="B31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="6"/>
+      <c r="E31" s="7"/>
+      <c r="H31" s="6"/>
+      <c r="J31" s="7"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O31" s="7"/>
+      <c r="Q31" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17">
+      <c r="C32" s="6"/>
+      <c r="E32" s="7"/>
+      <c r="H32" s="6"/>
+      <c r="J32" s="7"/>
+      <c r="M32" s="6"/>
+      <c r="O32" s="7"/>
+    </row>
+    <row r="33" spans="3:15">
+      <c r="C33" s="6"/>
+      <c r="E33" s="7"/>
+      <c r="H33" s="6"/>
+      <c r="J33" s="7"/>
+      <c r="M33" s="6"/>
+      <c r="O33" s="7"/>
+    </row>
+    <row r="34" spans="3:15">
+      <c r="C34" s="6"/>
+      <c r="E34" s="7"/>
+      <c r="H34" s="6"/>
+      <c r="J34" s="7"/>
+      <c r="M34" s="6"/>
+      <c r="O34" s="7"/>
+    </row>
+    <row r="35" spans="3:15">
+      <c r="C35" s="6"/>
+      <c r="E35" s="7"/>
+      <c r="H35" s="6"/>
+      <c r="J35" s="7"/>
+      <c r="M35" s="6"/>
+      <c r="O35" s="7"/>
+    </row>
+    <row r="36" spans="3:15">
+      <c r="C36" s="6"/>
+      <c r="E36" s="7"/>
+      <c r="H36" s="6"/>
+      <c r="J36" s="7"/>
+      <c r="M36" s="6"/>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="3:15">
+      <c r="C37" s="6"/>
+      <c r="E37" s="7"/>
+      <c r="H37" s="6"/>
+      <c r="J37" s="7"/>
+      <c r="M37" s="6"/>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="3:15">
+      <c r="C38" s="6"/>
+      <c r="E38" s="7"/>
+      <c r="H38" s="6"/>
+      <c r="J38" s="7"/>
+      <c r="M38" s="6"/>
+      <c r="O38" s="7"/>
+    </row>
+    <row r="39" spans="3:15" ht="14" thickBot="1">
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="11"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="11"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:G13"/>
   <sheetViews>
@@ -10337,7 +10768,7 @@
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="212" t="s">
+      <c r="B5" s="213" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -10357,7 +10788,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="212"/>
+      <c r="B6" s="213"/>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
@@ -10373,7 +10804,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="212"/>
+      <c r="B7" s="213"/>
       <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
@@ -10391,7 +10822,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="212"/>
+      <c r="B8" s="213"/>
       <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
@@ -10409,7 +10840,7 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="212"/>
+      <c r="B9" s="213"/>
       <c r="C9" s="16" t="s">
         <v>33</v>
       </c>
@@ -10427,7 +10858,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="28">
-      <c r="B10" s="212"/>
+      <c r="B10" s="213"/>
       <c r="C10" s="16" t="s">
         <v>13</v>
       </c>
@@ -10445,7 +10876,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="42">
-      <c r="B11" s="213" t="s">
+      <c r="B11" s="214" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -10465,7 +10896,7 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="214"/>
+      <c r="B12" s="215"/>
       <c r="C12" s="15" t="s">
         <v>15</v>
       </c>
@@ -10479,7 +10910,7 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="215"/>
+      <c r="B13" s="216"/>
       <c r="C13" s="15" t="s">
         <v>16</v>
       </c>
@@ -10505,7 +10936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:N24"/>
   <sheetViews>
@@ -10665,7 +11096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:U32"/>
   <sheetViews>
@@ -10926,7 +11357,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA80C652-EB11-2747-89DA-E4ABA79A811D}">
   <dimension ref="A2:T38"/>
   <sheetViews>
@@ -11035,11 +11466,11 @@
       <c r="C6" s="94"/>
       <c r="D6" s="101"/>
       <c r="E6" s="96"/>
-      <c r="F6" s="216" t="s">
+      <c r="F6" s="217" t="s">
         <v>392</v>
       </c>
-      <c r="G6" s="217"/>
-      <c r="H6" s="218"/>
+      <c r="G6" s="218"/>
+      <c r="H6" s="219"/>
       <c r="I6" s="96"/>
       <c r="J6" s="102"/>
       <c r="K6" s="94"/>
@@ -11059,9 +11490,9 @@
       <c r="C7" s="94"/>
       <c r="D7" s="101"/>
       <c r="E7" s="96"/>
-      <c r="F7" s="219"/>
-      <c r="G7" s="220"/>
-      <c r="H7" s="221"/>
+      <c r="F7" s="220"/>
+      <c r="G7" s="221"/>
+      <c r="H7" s="222"/>
       <c r="I7" s="96"/>
       <c r="J7" s="102"/>
       <c r="K7" s="95"/>
@@ -11081,9 +11512,9 @@
       <c r="C8" s="94"/>
       <c r="D8" s="101"/>
       <c r="E8" s="96"/>
-      <c r="F8" s="219"/>
-      <c r="G8" s="220"/>
-      <c r="H8" s="221"/>
+      <c r="F8" s="220"/>
+      <c r="G8" s="221"/>
+      <c r="H8" s="222"/>
       <c r="I8" s="96"/>
       <c r="J8" s="102"/>
       <c r="K8" s="94"/>
@@ -11102,9 +11533,9 @@
       <c r="B9" s="94"/>
       <c r="C9" s="94"/>
       <c r="D9" s="101"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="220"/>
-      <c r="H9" s="221"/>
+      <c r="F9" s="220"/>
+      <c r="G9" s="221"/>
+      <c r="H9" s="222"/>
       <c r="I9" s="96"/>
       <c r="J9" s="102"/>
       <c r="K9" s="94"/>
@@ -11123,9 +11554,9 @@
       <c r="B10" s="94"/>
       <c r="C10" s="94"/>
       <c r="D10" s="101"/>
-      <c r="F10" s="222"/>
-      <c r="G10" s="223"/>
-      <c r="H10" s="224"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="224"/>
+      <c r="H10" s="225"/>
       <c r="I10" s="129"/>
       <c r="J10" s="102"/>
       <c r="K10" s="94"/>
@@ -11718,7 +12149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7778B8-D430-A34A-995E-0F83AC473C52}">
   <dimension ref="E8:K35"/>
   <sheetViews>
@@ -11798,16 +12229,16 @@
     </row>
     <row r="18" spans="5:8">
       <c r="E18" s="137"/>
-      <c r="F18" s="225" t="s">
+      <c r="F18" s="226" t="s">
         <v>395</v>
       </c>
-      <c r="G18" s="226"/>
+      <c r="G18" s="227"/>
       <c r="H18" s="135"/>
     </row>
     <row r="19" spans="5:8">
       <c r="E19" s="137"/>
-      <c r="F19" s="227"/>
-      <c r="G19" s="228"/>
+      <c r="F19" s="228"/>
+      <c r="G19" s="229"/>
       <c r="H19" s="135"/>
     </row>
     <row r="20" spans="5:8">
@@ -11904,7 +12335,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B1:K25"/>
   <sheetViews>
@@ -12119,7 +12550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A3:E21"/>
   <sheetViews>
@@ -12302,7 +12733,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDFDE749-2C0C-C548-8C4F-6EF43EA89AA0}">
   <dimension ref="B2:C9"/>
   <sheetViews>
@@ -12381,7 +12812,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D86ED6A2-BD47-244B-AD18-088367512271}">
   <dimension ref="B2:M10"/>
   <sheetViews>
@@ -12486,7 +12917,163 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133A9786-8ADA-8C47-8004-675DACA89322}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="233" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="235"/>
+      <c r="C2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" s="237"/>
+      <c r="C3" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="232" customFormat="1">
+      <c r="B6" s="232" t="s">
+        <v>565</v>
+      </c>
+      <c r="E6" s="232" t="s">
+        <v>571</v>
+      </c>
+      <c r="H6" s="232" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="232" customFormat="1">
+      <c r="B7" s="236" t="s">
+        <v>566</v>
+      </c>
+      <c r="C7" s="236" t="s">
+        <v>567</v>
+      </c>
+      <c r="E7" s="234" t="s">
+        <v>572</v>
+      </c>
+      <c r="F7" s="234" t="s">
+        <v>573</v>
+      </c>
+      <c r="H7" s="236" t="s">
+        <v>566</v>
+      </c>
+      <c r="I7" s="236" t="s">
+        <v>572</v>
+      </c>
+      <c r="J7" s="236" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" s="159">
+        <v>1</v>
+      </c>
+      <c r="C8" s="150" t="s">
+        <v>568</v>
+      </c>
+      <c r="E8" s="150">
+        <v>1</v>
+      </c>
+      <c r="F8" s="150" t="s">
+        <v>577</v>
+      </c>
+      <c r="H8" s="150">
+        <v>1</v>
+      </c>
+      <c r="I8" s="150">
+        <v>1</v>
+      </c>
+      <c r="J8" s="150">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="159">
+        <v>2</v>
+      </c>
+      <c r="C9" s="150" t="s">
+        <v>576</v>
+      </c>
+      <c r="E9" s="150">
+        <v>2</v>
+      </c>
+      <c r="F9" s="150" t="s">
+        <v>578</v>
+      </c>
+      <c r="H9" s="150">
+        <v>1</v>
+      </c>
+      <c r="I9" s="150">
+        <v>1</v>
+      </c>
+      <c r="J9" s="150">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="235"/>
+      <c r="E10" s="235"/>
+      <c r="H10" s="150">
+        <v>2</v>
+      </c>
+      <c r="I10" s="150">
+        <v>2</v>
+      </c>
+      <c r="J10" s="150">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="H11" s="150">
+        <v>2</v>
+      </c>
+      <c r="I11" s="150">
+        <v>2</v>
+      </c>
+      <c r="J11" s="150">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="H12" s="238"/>
+      <c r="I12" s="235"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="H13" s="237"/>
+      <c r="I13" s="93"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="I14" s="237"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Home!B4" display="Home" xr:uid="{514B2CEF-E7A5-864D-80CF-0C54175C6FEA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A51D4780-106D-3C46-B51D-1FAF5E0D4E2A}">
   <dimension ref="A1:K27"/>
   <sheetViews>
@@ -12754,11 +13341,205 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C5F8E-5AB4-3747-B9CF-9A1C944F7742}">
+  <dimension ref="A1:I35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="152" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="147" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="F5" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="F6" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="I9" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="F10" s="230"/>
+      <c r="G10" s="230"/>
+      <c r="I10" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="G13" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" t="s">
+        <v>441</v>
+      </c>
+      <c r="F17" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="F22" s="149"/>
+      <c r="G22" s="149"/>
+      <c r="I22" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="G24" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="F28" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="F32" s="230"/>
+      <c r="G32" s="230"/>
+      <c r="I32" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9">
+      <c r="I33" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9">
+      <c r="G35" t="s">
+        <v>439</v>
+      </c>
+      <c r="I35" t="s">
+        <v>449</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F32:G32"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{8C105A6D-028F-7B45-AB3A-0ACED100F9CD}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{DECB92E9-F7C3-7E48-B60C-768E77C89B1F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE8B8C4-352E-054D-A843-45DFD254B784}">
+  <dimension ref="B2:J61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="H2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="H12" s="231" t="s">
+        <v>399</v>
+      </c>
+      <c r="I12" s="231"/>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="J14" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="H28" s="230" t="s">
+        <v>403</v>
+      </c>
+      <c r="I28" s="230"/>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="H43" s="231" t="s">
+        <v>406</v>
+      </c>
+      <c r="I43" s="231"/>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="B54" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9">
+      <c r="H59" s="230" t="s">
+        <v>403</v>
+      </c>
+      <c r="I59" s="230"/>
+    </row>
+    <row r="61" spans="2:9">
+      <c r="G61" t="s">
+        <v>405</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="H59:I59"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3066BC90-58A1-734D-AE58-036202455225}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -12859,7 +13640,7 @@
       <c r="F7" s="144" t="s">
         <v>548</v>
       </c>
-      <c r="G7" s="231" t="s">
+      <c r="G7" s="210" t="s">
         <v>548</v>
       </c>
     </row>
@@ -12899,7 +13680,7 @@
       <c r="F9" s="144" t="s">
         <v>537</v>
       </c>
-      <c r="G9" s="231" t="s">
+      <c r="G9" s="210" t="s">
         <v>559</v>
       </c>
     </row>
@@ -12930,201 +13711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112C5F8E-5AB4-3747-B9CF-9A1C944F7742}">
-  <dimension ref="A1:I35"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="152" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="147" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="F5" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="F6" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="I9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="F10" s="229"/>
-      <c r="G10" s="229"/>
-      <c r="I10" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="G13" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="B17" t="s">
-        <v>441</v>
-      </c>
-      <c r="F17" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9">
-      <c r="F22" s="149"/>
-      <c r="G22" s="149"/>
-      <c r="I22" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9">
-      <c r="G24" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9">
-      <c r="F28" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9">
-      <c r="F32" s="229"/>
-      <c r="G32" s="229"/>
-      <c r="I32" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="33" spans="7:9">
-      <c r="I33" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="35" spans="7:9">
-      <c r="G35" t="s">
-        <v>439</v>
-      </c>
-      <c r="I35" t="s">
-        <v>449</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F32:G32"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{8C105A6D-028F-7B45-AB3A-0ACED100F9CD}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{DECB92E9-F7C3-7E48-B60C-768E77C89B1F}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDE8B8C4-352E-054D-A843-45DFD254B784}">
-  <dimension ref="B2:J61"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
-  <sheetData>
-    <row r="2" spans="2:10">
-      <c r="H2" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="H12" s="230" t="s">
-        <v>399</v>
-      </c>
-      <c r="I12" s="230"/>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="J14" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9">
-      <c r="B23" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9">
-      <c r="H28" s="229" t="s">
-        <v>403</v>
-      </c>
-      <c r="I28" s="229"/>
-    </row>
-    <row r="39" spans="2:9">
-      <c r="B39" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="43" spans="2:9">
-      <c r="H43" s="230" t="s">
-        <v>406</v>
-      </c>
-      <c r="I43" s="230"/>
-    </row>
-    <row r="54" spans="2:9">
-      <c r="B54" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="59" spans="2:9">
-      <c r="H59" s="229" t="s">
-        <v>403</v>
-      </c>
-      <c r="I59" s="229"/>
-    </row>
-    <row r="61" spans="2:9">
-      <c r="G61" t="s">
-        <v>405</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="H59:I59"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E51BCB48-68B0-EF46-B93E-648BAB230ADA}">
   <dimension ref="A1:S28"/>
   <sheetViews>
@@ -13428,7 +14015,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0C945C-04F2-D147-89E5-6DDFCFB3EEA7}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -13451,13 +14038,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="210" t="s">
+      <c r="A2" s="211" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="210"/>
-      <c r="C2" s="210"/>
-      <c r="D2" s="210"/>
-      <c r="E2" s="210"/>
+      <c r="B2" s="211"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="143" t="s">
@@ -13596,7 +14183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{695F25B9-FD59-DD4E-A097-058E28B48012}">
   <dimension ref="A1:G19"/>
   <sheetViews>
@@ -13610,15 +14197,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="211" t="s">
+      <c r="A1" s="212" t="s">
         <v>434</v>
       </c>
-      <c r="B1" s="211"/>
-      <c r="C1" s="211"/>
-      <c r="D1" s="211"/>
-      <c r="E1" s="211"/>
-      <c r="F1" s="211"/>
-      <c r="G1" s="211"/>
+      <c r="B1" s="212"/>
+      <c r="C1" s="212"/>
+      <c r="D1" s="212"/>
+      <c r="E1" s="212"/>
+      <c r="F1" s="212"/>
+      <c r="G1" s="212"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="143" t="s">
@@ -13728,15 +14315,15 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="211" t="s">
+      <c r="A12" s="212" t="s">
         <v>433</v>
       </c>
-      <c r="B12" s="211"/>
-      <c r="C12" s="211"/>
-      <c r="D12" s="211"/>
-      <c r="E12" s="211"/>
-      <c r="F12" s="211"/>
-      <c r="G12" s="211"/>
+      <c r="B12" s="212"/>
+      <c r="C12" s="212"/>
+      <c r="D12" s="212"/>
+      <c r="E12" s="212"/>
+      <c r="F12" s="212"/>
+      <c r="G12" s="212"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="143" t="s">
@@ -13855,7 +14442,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:Q30"/>
   <sheetViews>
@@ -14271,7 +14858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D224"/>
@@ -16252,7 +16839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:I20"/>
   <sheetViews>
@@ -16364,335 +16951,4 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:Q39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J46" sqref="J46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>
-  <cols>
-    <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16" width="9" style="1"/>
-    <col min="17" max="17" width="68.6640625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:17">
-      <c r="C1" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="2:17" ht="14" thickBot="1">
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17">
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="2:17">
-      <c r="C4" s="6"/>
-      <c r="E4" s="7"/>
-      <c r="H4" s="6"/>
-      <c r="J4" s="7"/>
-      <c r="M4" s="6"/>
-      <c r="O4" s="7"/>
-    </row>
-    <row r="5" spans="2:17">
-      <c r="C5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="H5" s="6"/>
-      <c r="J5" s="7"/>
-      <c r="M5" s="6"/>
-      <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="2:17">
-      <c r="C6" s="6"/>
-      <c r="E6" s="7"/>
-      <c r="H6" s="6"/>
-      <c r="J6" s="7"/>
-      <c r="M6" s="6"/>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="2:17">
-      <c r="C7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="J7" s="7"/>
-      <c r="M7" s="6"/>
-      <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="2:17" ht="14" thickBot="1">
-      <c r="C8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="J8" s="7"/>
-      <c r="M8" s="6"/>
-      <c r="O8" s="7"/>
-    </row>
-    <row r="9" spans="2:17" ht="29" thickBot="1">
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="7"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O9" s="7"/>
-      <c r="Q9" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17">
-      <c r="C10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="H10" s="6"/>
-      <c r="J10" s="7"/>
-      <c r="M10" s="6"/>
-      <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="2:17">
-      <c r="C11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="H11" s="6"/>
-      <c r="J11" s="7"/>
-      <c r="M11" s="6"/>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="2:17">
-      <c r="C12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="H12" s="6"/>
-      <c r="J12" s="7"/>
-      <c r="M12" s="6"/>
-      <c r="O12" s="7"/>
-    </row>
-    <row r="13" spans="2:17">
-      <c r="C13" s="6"/>
-      <c r="E13" s="7"/>
-      <c r="H13" s="6"/>
-      <c r="J13" s="7"/>
-      <c r="M13" s="6"/>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="2:17">
-      <c r="C14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="H14" s="6"/>
-      <c r="J14" s="7"/>
-      <c r="M14" s="6"/>
-      <c r="O14" s="7"/>
-    </row>
-    <row r="15" spans="2:17">
-      <c r="C15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="H15" s="6"/>
-      <c r="J15" s="7"/>
-      <c r="M15" s="6"/>
-      <c r="O15" s="7"/>
-    </row>
-    <row r="16" spans="2:17">
-      <c r="C16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="H16" s="6"/>
-      <c r="J16" s="7"/>
-      <c r="M16" s="6"/>
-      <c r="O16" s="7"/>
-    </row>
-    <row r="17" spans="2:17" ht="14" thickBot="1">
-      <c r="C17" s="9"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="11"/>
-    </row>
-    <row r="24" spans="2:17" ht="14" thickBot="1">
-      <c r="D24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17">
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="5"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="5"/>
-      <c r="M25" s="3"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="5"/>
-    </row>
-    <row r="26" spans="2:17">
-      <c r="C26" s="6"/>
-      <c r="E26" s="7"/>
-      <c r="H26" s="6"/>
-      <c r="J26" s="7"/>
-      <c r="M26" s="6"/>
-      <c r="O26" s="7"/>
-    </row>
-    <row r="27" spans="2:17">
-      <c r="C27" s="6"/>
-      <c r="E27" s="7"/>
-      <c r="H27" s="6"/>
-      <c r="J27" s="7"/>
-      <c r="M27" s="6"/>
-      <c r="O27" s="7"/>
-    </row>
-    <row r="28" spans="2:17">
-      <c r="C28" s="6"/>
-      <c r="E28" s="7"/>
-      <c r="H28" s="6"/>
-      <c r="J28" s="7"/>
-      <c r="M28" s="6"/>
-      <c r="O28" s="7"/>
-    </row>
-    <row r="29" spans="2:17">
-      <c r="C29" s="6"/>
-      <c r="E29" s="7"/>
-      <c r="H29" s="6"/>
-      <c r="J29" s="7"/>
-      <c r="M29" s="6"/>
-      <c r="O29" s="7"/>
-    </row>
-    <row r="30" spans="2:17">
-      <c r="C30" s="6"/>
-      <c r="E30" s="7"/>
-      <c r="H30" s="6"/>
-      <c r="J30" s="7"/>
-      <c r="M30" s="6"/>
-      <c r="O30" s="7"/>
-    </row>
-    <row r="31" spans="2:17" ht="42">
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="E31" s="7"/>
-      <c r="H31" s="6"/>
-      <c r="J31" s="7"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="O31" s="7"/>
-      <c r="Q31" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17">
-      <c r="C32" s="6"/>
-      <c r="E32" s="7"/>
-      <c r="H32" s="6"/>
-      <c r="J32" s="7"/>
-      <c r="M32" s="6"/>
-      <c r="O32" s="7"/>
-    </row>
-    <row r="33" spans="3:15">
-      <c r="C33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="H33" s="6"/>
-      <c r="J33" s="7"/>
-      <c r="M33" s="6"/>
-      <c r="O33" s="7"/>
-    </row>
-    <row r="34" spans="3:15">
-      <c r="C34" s="6"/>
-      <c r="E34" s="7"/>
-      <c r="H34" s="6"/>
-      <c r="J34" s="7"/>
-      <c r="M34" s="6"/>
-      <c r="O34" s="7"/>
-    </row>
-    <row r="35" spans="3:15">
-      <c r="C35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="H35" s="6"/>
-      <c r="J35" s="7"/>
-      <c r="M35" s="6"/>
-      <c r="O35" s="7"/>
-    </row>
-    <row r="36" spans="3:15">
-      <c r="C36" s="6"/>
-      <c r="E36" s="7"/>
-      <c r="H36" s="6"/>
-      <c r="J36" s="7"/>
-      <c r="M36" s="6"/>
-      <c r="O36" s="7"/>
-    </row>
-    <row r="37" spans="3:15">
-      <c r="C37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="H37" s="6"/>
-      <c r="J37" s="7"/>
-      <c r="M37" s="6"/>
-      <c r="O37" s="7"/>
-    </row>
-    <row r="38" spans="3:15">
-      <c r="C38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="H38" s="6"/>
-      <c r="J38" s="7"/>
-      <c r="M38" s="6"/>
-      <c r="O38" s="7"/>
-    </row>
-    <row r="39" spans="3:15" ht="14" thickBot="1">
-      <c r="C39" s="9"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="11"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="11"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="11"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
test attrs can use in xml
</commit_message>
<xml_diff>
--- a/doc/android.xlsx
+++ b/doc/android.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F244A371-D644-6C42-A369-1B2235AD3724}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F209B1D-B3E2-5146-9D82-A491727E662D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="460" windowWidth="27840" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="588">
   <si>
     <t>Activity</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2308,12 +2308,44 @@
     <t>Harvard</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>@Insert long[] insertScores(Score score1, Score score2);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>@Insert List&lt;Long&gt; insertScores(List&lt;Score&gt; scores);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>@Insert long[] insertScores(Score score1, List&lt;Score&gt; scores);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9条数据</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>@Insert(onConflict = OnConflictStrategy.REPLACE) void insertCourses(Course... courses)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>@Insert long insertStudent(Student student)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>@Insert long[] insertStudents(List&lt;Student&gt; students);</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>temp</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="46">
+  <fonts count="49">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2654,8 +2686,32 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2722,8 +2778,23 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="64">
+  <borders count="66">
     <border>
       <left/>
       <right/>
@@ -3432,13 +3503,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="244">
+  <cellXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3841,6 +3945,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="42" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="12" borderId="0" xfId="3" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="14" borderId="0" xfId="5" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="13" borderId="64" xfId="4" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="13" borderId="0" xfId="4" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="12" borderId="0" xfId="3" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="47" fillId="13" borderId="10" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3904,24 +4043,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="13" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{66AFF3AD-B4DE-FA4E-AB57-26B45159E82C}"/>
   </cellStyles>
@@ -10347,7 +10495,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -10782,7 +10930,7 @@
       <c r="G4" s="15"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="220" t="s">
+      <c r="B5" s="233" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="15" t="s">
@@ -10802,7 +10950,7 @@
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="220"/>
+      <c r="B6" s="233"/>
       <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
@@ -10818,7 +10966,7 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="220"/>
+      <c r="B7" s="233"/>
       <c r="C7" s="16" t="s">
         <v>31</v>
       </c>
@@ -10836,7 +10984,7 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="220"/>
+      <c r="B8" s="233"/>
       <c r="C8" s="16" t="s">
         <v>32</v>
       </c>
@@ -10854,7 +11002,7 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="220"/>
+      <c r="B9" s="233"/>
       <c r="C9" s="16" t="s">
         <v>33</v>
       </c>
@@ -10872,7 +11020,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="28">
-      <c r="B10" s="220"/>
+      <c r="B10" s="233"/>
       <c r="C10" s="16" t="s">
         <v>13</v>
       </c>
@@ -10890,7 +11038,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="42">
-      <c r="B11" s="221" t="s">
+      <c r="B11" s="234" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -10910,7 +11058,7 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="222"/>
+      <c r="B12" s="235"/>
       <c r="C12" s="15" t="s">
         <v>15</v>
       </c>
@@ -10924,7 +11072,7 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="223"/>
+      <c r="B13" s="236"/>
       <c r="C13" s="15" t="s">
         <v>16</v>
       </c>
@@ -11480,11 +11628,11 @@
       <c r="C6" s="94"/>
       <c r="D6" s="101"/>
       <c r="E6" s="96"/>
-      <c r="F6" s="224" t="s">
+      <c r="F6" s="237" t="s">
         <v>392</v>
       </c>
-      <c r="G6" s="225"/>
-      <c r="H6" s="226"/>
+      <c r="G6" s="238"/>
+      <c r="H6" s="239"/>
       <c r="I6" s="96"/>
       <c r="J6" s="102"/>
       <c r="K6" s="94"/>
@@ -11504,9 +11652,9 @@
       <c r="C7" s="94"/>
       <c r="D7" s="101"/>
       <c r="E7" s="96"/>
-      <c r="F7" s="227"/>
-      <c r="G7" s="228"/>
-      <c r="H7" s="229"/>
+      <c r="F7" s="240"/>
+      <c r="G7" s="241"/>
+      <c r="H7" s="242"/>
       <c r="I7" s="96"/>
       <c r="J7" s="102"/>
       <c r="K7" s="95"/>
@@ -11526,9 +11674,9 @@
       <c r="C8" s="94"/>
       <c r="D8" s="101"/>
       <c r="E8" s="96"/>
-      <c r="F8" s="227"/>
-      <c r="G8" s="228"/>
-      <c r="H8" s="229"/>
+      <c r="F8" s="240"/>
+      <c r="G8" s="241"/>
+      <c r="H8" s="242"/>
       <c r="I8" s="96"/>
       <c r="J8" s="102"/>
       <c r="K8" s="94"/>
@@ -11547,9 +11695,9 @@
       <c r="B9" s="94"/>
       <c r="C9" s="94"/>
       <c r="D9" s="101"/>
-      <c r="F9" s="227"/>
-      <c r="G9" s="228"/>
-      <c r="H9" s="229"/>
+      <c r="F9" s="240"/>
+      <c r="G9" s="241"/>
+      <c r="H9" s="242"/>
       <c r="I9" s="96"/>
       <c r="J9" s="102"/>
       <c r="K9" s="94"/>
@@ -11568,9 +11716,9 @@
       <c r="B10" s="94"/>
       <c r="C10" s="94"/>
       <c r="D10" s="101"/>
-      <c r="F10" s="230"/>
-      <c r="G10" s="231"/>
-      <c r="H10" s="232"/>
+      <c r="F10" s="243"/>
+      <c r="G10" s="244"/>
+      <c r="H10" s="245"/>
       <c r="I10" s="129"/>
       <c r="J10" s="102"/>
       <c r="K10" s="94"/>
@@ -12243,16 +12391,16 @@
     </row>
     <row r="18" spans="5:8">
       <c r="E18" s="137"/>
-      <c r="F18" s="233" t="s">
+      <c r="F18" s="246" t="s">
         <v>395</v>
       </c>
-      <c r="G18" s="234"/>
+      <c r="G18" s="247"/>
       <c r="H18" s="135"/>
     </row>
     <row r="19" spans="5:8">
       <c r="E19" s="137"/>
-      <c r="F19" s="235"/>
-      <c r="G19" s="236"/>
+      <c r="F19" s="248"/>
+      <c r="G19" s="249"/>
       <c r="H19" s="135"/>
     </row>
     <row r="20" spans="5:8">
@@ -12933,228 +13081,331 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{133A9786-8ADA-8C47-8004-675DACA89322}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" style="217" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="112" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:7">
       <c r="A1" s="212" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:7">
       <c r="B2" s="214"/>
       <c r="C2" s="217" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:7">
       <c r="B3" s="216"/>
       <c r="C3" s="217" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:7">
       <c r="B5" s="211" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="211" customFormat="1">
-      <c r="C6" s="242"/>
-    </row>
-    <row r="7" spans="1:3" s="211" customFormat="1">
-      <c r="B7" s="239" t="s">
+    <row r="6" spans="1:7" s="211" customFormat="1">
+      <c r="C6" s="221"/>
+    </row>
+    <row r="7" spans="1:7" s="211" customFormat="1">
+      <c r="B7" s="218" t="s">
         <v>566</v>
       </c>
       <c r="C7" s="215" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:7" ht="16">
       <c r="B8" s="159">
         <v>1</v>
       </c>
       <c r="C8" s="150" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="G8" s="227" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16">
       <c r="B9" s="159">
         <v>2</v>
       </c>
       <c r="C9" s="150" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="G9" s="227" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10" s="93"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:7">
       <c r="B12" s="211" t="s">
         <v>571</v>
       </c>
-      <c r="C12" s="242"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" s="239" t="s">
+      <c r="C12" s="221"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="218" t="s">
         <v>572</v>
       </c>
       <c r="C13" s="213" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:7" ht="16">
       <c r="B14" s="150">
         <v>1</v>
       </c>
-      <c r="C14" s="240" t="s">
+      <c r="C14" s="219" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="G14" s="227" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15">
       <c r="B15" s="150">
         <v>2</v>
       </c>
-      <c r="C15" s="240" t="s">
+      <c r="C15" s="219" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="G15" s="228" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15">
       <c r="B16" s="159">
         <v>3</v>
       </c>
       <c r="C16" s="150" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="19" spans="2:4">
+      <c r="G16" s="228" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
       <c r="B19" s="211" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:7">
       <c r="B20" s="216"/>
-      <c r="C20" s="243"/>
+      <c r="C20" s="222"/>
       <c r="D20" s="211"/>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21" s="239" t="s">
+      <c r="E20" s="211"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="218" t="s">
         <v>566</v>
       </c>
-      <c r="C21" s="239" t="s">
+      <c r="C21" s="218" t="s">
         <v>572</v>
       </c>
       <c r="D21" s="215" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22" s="150">
+      <c r="E21" s="253" t="s">
+        <v>587</v>
+      </c>
+      <c r="F21" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="16">
+      <c r="B22" s="230">
         <v>1</v>
       </c>
-      <c r="C22" s="150">
+      <c r="C22" s="230">
         <v>1</v>
       </c>
-      <c r="D22" s="150">
+      <c r="D22" s="230">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23" s="150">
+      <c r="E22" s="254">
         <v>1</v>
       </c>
-      <c r="C23" s="150">
+      <c r="F22" s="223">
+        <v>1</v>
+      </c>
+      <c r="G22" s="224" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="16">
+      <c r="B23" s="230">
+        <v>1</v>
+      </c>
+      <c r="C23" s="230">
         <v>2</v>
       </c>
-      <c r="D23" s="150">
+      <c r="D23" s="230">
         <v>97</v>
       </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24" s="150">
+      <c r="E23" s="254">
+        <v>2</v>
+      </c>
+      <c r="F23" s="223">
+        <v>2</v>
+      </c>
+      <c r="G23" s="224" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="16">
+      <c r="B24" s="252">
         <v>1</v>
       </c>
-      <c r="C24" s="150">
+      <c r="C24" s="252">
         <v>3</v>
       </c>
-      <c r="D24" s="150">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25" s="150">
+      <c r="D24" s="252">
+        <v>75</v>
+      </c>
+      <c r="E24" s="255">
         <v>2</v>
       </c>
-      <c r="C25" s="150">
+      <c r="F24" s="223">
+        <v>3</v>
+      </c>
+      <c r="G24" s="225" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="16">
+      <c r="B25" s="252">
+        <v>2</v>
+      </c>
+      <c r="C25" s="252">
         <v>1</v>
       </c>
-      <c r="D25" s="150">
+      <c r="D25" s="252">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26" s="150">
+      <c r="E25" s="256">
+        <v>4</v>
+      </c>
+      <c r="F25" s="185">
+        <v>4</v>
+      </c>
+      <c r="G25" s="225" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="15">
+      <c r="B26" s="252">
         <v>2</v>
       </c>
-      <c r="C26" s="150">
+      <c r="C26" s="252">
         <v>2</v>
       </c>
-      <c r="D26" s="150">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27" s="241">
+      <c r="D26" s="252">
+        <v>60</v>
+      </c>
+      <c r="E26" s="256">
+        <v>5</v>
+      </c>
+      <c r="F26" s="185">
+        <v>5</v>
+      </c>
+      <c r="G26" s="226" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="15">
+      <c r="B27" s="220">
         <v>2</v>
       </c>
-      <c r="C27" s="241">
+      <c r="C27" s="220">
         <v>3</v>
       </c>
-      <c r="D27" s="159">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28" s="241">
+      <c r="D27" s="220">
+        <v>85</v>
+      </c>
+      <c r="E27" s="257">
+        <v>6</v>
+      </c>
+      <c r="F27" s="185">
+        <v>6</v>
+      </c>
+      <c r="G27" s="226" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="15">
+      <c r="B28" s="229">
         <v>3</v>
       </c>
-      <c r="C28" s="241">
+      <c r="C28" s="229">
         <v>1</v>
       </c>
-      <c r="D28" s="159">
+      <c r="D28" s="229">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29" s="241">
+      <c r="E28" s="258">
+        <v>7</v>
+      </c>
+      <c r="F28" s="185">
+        <v>7</v>
+      </c>
+      <c r="G28" s="226" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="15">
+      <c r="B29" s="229">
         <v>3</v>
       </c>
-      <c r="C29" s="241">
+      <c r="C29" s="229">
         <v>2</v>
       </c>
-      <c r="D29" s="159">
+      <c r="D29" s="229">
         <v>95</v>
       </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30" s="241">
+      <c r="E29" s="258">
+        <v>8</v>
+      </c>
+      <c r="F29" s="185">
+        <v>8</v>
+      </c>
+      <c r="G29" s="226" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="15">
+      <c r="B30" s="229">
         <v>3</v>
       </c>
-      <c r="C30" s="241">
+      <c r="C30" s="229">
         <v>3</v>
       </c>
-      <c r="D30" s="159">
+      <c r="D30" s="229">
         <v>75</v>
+      </c>
+      <c r="E30" s="258">
+        <v>9</v>
+      </c>
+      <c r="F30" s="185">
+        <v>9</v>
+      </c>
+      <c r="G30" s="226" t="s">
+        <v>582</v>
       </c>
     </row>
   </sheetData>
@@ -13471,8 +13722,8 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="F10" s="237"/>
-      <c r="G10" s="237"/>
+      <c r="F10" s="250"/>
+      <c r="G10" s="250"/>
       <c r="I10" t="s">
         <v>445</v>
       </c>
@@ -13513,8 +13764,8 @@
       </c>
     </row>
     <row r="32" spans="2:9">
-      <c r="F32" s="237"/>
-      <c r="G32" s="237"/>
+      <c r="F32" s="250"/>
+      <c r="G32" s="250"/>
       <c r="I32" t="s">
         <v>442</v>
       </c>
@@ -13568,10 +13819,10 @@
       </c>
     </row>
     <row r="12" spans="2:10">
-      <c r="H12" s="238" t="s">
+      <c r="H12" s="251" t="s">
         <v>399</v>
       </c>
-      <c r="I12" s="238"/>
+      <c r="I12" s="251"/>
     </row>
     <row r="14" spans="2:10">
       <c r="J14" t="s">
@@ -13584,10 +13835,10 @@
       </c>
     </row>
     <row r="28" spans="2:9">
-      <c r="H28" s="237" t="s">
+      <c r="H28" s="250" t="s">
         <v>403</v>
       </c>
-      <c r="I28" s="237"/>
+      <c r="I28" s="250"/>
     </row>
     <row r="39" spans="2:9">
       <c r="B39" t="s">
@@ -13595,10 +13846,10 @@
       </c>
     </row>
     <row r="43" spans="2:9">
-      <c r="H43" s="238" t="s">
+      <c r="H43" s="251" t="s">
         <v>406</v>
       </c>
-      <c r="I43" s="238"/>
+      <c r="I43" s="251"/>
     </row>
     <row r="54" spans="2:9">
       <c r="B54" t="s">
@@ -13606,10 +13857,10 @@
       </c>
     </row>
     <row r="59" spans="2:9">
-      <c r="H59" s="237" t="s">
+      <c r="H59" s="250" t="s">
         <v>403</v>
       </c>
-      <c r="I59" s="237"/>
+      <c r="I59" s="250"/>
     </row>
     <row r="61" spans="2:9">
       <c r="G61" t="s">
@@ -14132,13 +14383,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="218" t="s">
+      <c r="A2" s="231" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="218"/>
-      <c r="C2" s="218"/>
-      <c r="D2" s="218"/>
-      <c r="E2" s="218"/>
+      <c r="B2" s="231"/>
+      <c r="C2" s="231"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="231"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="143" t="s">
@@ -14291,15 +14542,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="232" t="s">
         <v>434</v>
       </c>
-      <c r="B1" s="219"/>
-      <c r="C1" s="219"/>
-      <c r="D1" s="219"/>
-      <c r="E1" s="219"/>
-      <c r="F1" s="219"/>
-      <c r="G1" s="219"/>
+      <c r="B1" s="232"/>
+      <c r="C1" s="232"/>
+      <c r="D1" s="232"/>
+      <c r="E1" s="232"/>
+      <c r="F1" s="232"/>
+      <c r="G1" s="232"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="143" t="s">
@@ -14409,15 +14660,15 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="219" t="s">
+      <c r="A12" s="232" t="s">
         <v>433</v>
       </c>
-      <c r="B12" s="219"/>
-      <c r="C12" s="219"/>
-      <c r="D12" s="219"/>
-      <c r="E12" s="219"/>
-      <c r="F12" s="219"/>
-      <c r="G12" s="219"/>
+      <c r="B12" s="232"/>
+      <c r="C12" s="232"/>
+      <c r="D12" s="232"/>
+      <c r="E12" s="232"/>
+      <c r="F12" s="232"/>
+      <c r="G12" s="232"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="143" t="s">

</xml_diff>